<commit_message>
* adding master design review spreadsheet
</commit_message>
<xml_diff>
--- a/docs/graviton_master.xlsx
+++ b/docs/graviton_master.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17055" windowHeight="12030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17055" windowHeight="12030" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="rx_chain" sheetId="1" r:id="rId1"/>
+    <sheet name="tx_chain" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t xml:space="preserve">Graviton Receiver Analog Front End Cascade Analysis </t>
   </si>
@@ -177,6 +178,39 @@
   </si>
   <si>
     <t>DSA (I.L. + setting)</t>
+  </si>
+  <si>
+    <t>output power (dBm)</t>
+  </si>
+  <si>
+    <t>amp3 (dB)</t>
+  </si>
+  <si>
+    <t>amp2 (dB)</t>
+  </si>
+  <si>
+    <t>saw2 (dB)</t>
+  </si>
+  <si>
+    <t>amp1 (dB)</t>
+  </si>
+  <si>
+    <t>saw1 (dB)</t>
+  </si>
+  <si>
+    <t>mixer (dB)</t>
+  </si>
+  <si>
+    <t>DAC out / mixer in (dBm)</t>
+  </si>
+  <si>
+    <t>GVA-84+</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>proposed</t>
   </si>
 </sst>
 </file>
@@ -186,7 +220,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -512,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -540,18 +574,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -596,10 +618,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -883,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AG52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,10 +955,10 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H2" s="28">
         <v>39000000</v>
       </c>
     </row>
@@ -926,103 +970,103 @@
         <v>1</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34" t="s">
+      <c r="I5" s="29"/>
+      <c r="J5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34" t="s">
+      <c r="L5" s="30"/>
+      <c r="M5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="34" t="s">
+      <c r="N5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="34" t="s">
+      <c r="O5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="34" t="s">
+      <c r="P5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="34" t="s">
+      <c r="Q5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="34" t="s">
+      <c r="R5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="33"/>
-      <c r="T5" s="34" t="s">
+      <c r="S5" s="29"/>
+      <c r="T5" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="U5" s="34" t="s">
+      <c r="U5" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="V5" s="34" t="s">
+      <c r="V5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="W5" s="34" t="s">
+      <c r="W5" s="30" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="45" t="s">
+      <c r="F6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34" t="s">
+      <c r="H6" s="34"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34" t="s">
+      <c r="L6" s="30"/>
+      <c r="M6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="34" t="s">
+      <c r="N6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="34" t="s">
+      <c r="O6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="34" t="s">
+      <c r="P6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="34" t="s">
+      <c r="Q6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="34" t="s">
+      <c r="R6" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="33"/>
-      <c r="T6" s="34" t="s">
+      <c r="S6" s="29"/>
+      <c r="T6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="34" t="s">
+      <c r="U6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="V6" s="34" t="s">
+      <c r="V6" s="30" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1033,7 +1077,7 @@
       <c r="E7" s="11">
         <v>0</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="42">
         <f>10^(E7/10)</f>
         <v>1</v>
       </c>
@@ -1062,11 +1106,11 @@
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="57">
+      <c r="Q7" s="53">
         <f t="shared" ref="Q7:Q18" si="1">Q8-E7</f>
         <v>-40.4</v>
       </c>
-      <c r="R7" s="59">
+      <c r="R7" s="55">
         <f>10^((Q7-30)/10)*1000000</f>
         <v>9.1201083935590621E-2</v>
       </c>
@@ -1078,11 +1122,11 @@
       <c r="E8" s="13">
         <v>-1</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="43">
         <f>10^(E8/10)</f>
         <v>0.79432823472428149</v>
       </c>
-      <c r="G8" s="51">
+      <c r="G8" s="47">
         <v>1</v>
       </c>
       <c r="H8" s="14">
@@ -1110,7 +1154,7 @@
         <f t="shared" si="1"/>
         <v>-40.4</v>
       </c>
-      <c r="R8" s="60">
+      <c r="R8" s="56">
         <f t="shared" ref="R8:R22" si="3">10^((Q8-30)/10)*1000000</f>
         <v>9.1201083935590621E-2</v>
       </c>
@@ -1126,11 +1170,11 @@
       <c r="E9" s="13">
         <v>0</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="39">
         <f t="shared" ref="F9:F22" si="4">10^(E9/10)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="51">
+      <c r="G9" s="47">
         <f>ABS(E9)</f>
         <v>0</v>
       </c>
@@ -1159,7 +1203,7 @@
         <f t="shared" si="1"/>
         <v>-41.4</v>
       </c>
-      <c r="R9" s="60">
+      <c r="R9" s="56">
         <f t="shared" si="3"/>
         <v>7.2443596007498792E-2</v>
       </c>
@@ -1175,11 +1219,11 @@
       <c r="E10" s="13">
         <v>0</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="39">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G10" s="51">
+      <c r="G10" s="47">
         <f>ABS(E10)</f>
         <v>0</v>
       </c>
@@ -1208,7 +1252,7 @@
         <f t="shared" si="1"/>
         <v>-41.4</v>
       </c>
-      <c r="R10" s="60">
+      <c r="R10" s="56">
         <f t="shared" si="3"/>
         <v>7.2443596007498792E-2</v>
       </c>
@@ -1221,18 +1265,18 @@
       <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="50" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="13">
         <v>18.399999999999999</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="39">
         <f t="shared" si="4"/>
         <v>69.183097091893657</v>
       </c>
-      <c r="G11" s="51">
+      <c r="G11" s="47">
         <v>0.27</v>
       </c>
       <c r="H11" s="14">
@@ -1262,11 +1306,11 @@
       <c r="P11">
         <v>-27.4</v>
       </c>
-      <c r="Q11" s="58">
+      <c r="Q11" s="54">
         <f>Q12-E11</f>
         <v>-41.4</v>
       </c>
-      <c r="R11" s="60">
+      <c r="R11" s="56">
         <f t="shared" si="3"/>
         <v>7.2443596007498792E-2</v>
       </c>
@@ -1286,18 +1330,18 @@
       <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="58" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="13">
         <v>-2</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="39">
         <f t="shared" ref="F12" si="9">10^(E12/10)</f>
         <v>0.63095734448019325</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="47">
         <f>ABS(E12)</f>
         <v>2</v>
       </c>
@@ -1326,7 +1370,7 @@
         <f t="shared" ref="Q12" si="14">Q13-E12</f>
         <v>-23</v>
       </c>
-      <c r="R12" s="60">
+      <c r="R12" s="56">
         <f t="shared" ref="R12" si="15">10^((Q12-30)/10)*1000000</f>
         <v>5.0118723362727193</v>
       </c>
@@ -1339,18 +1383,18 @@
       <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="50" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="15">
         <v>-1.5</v>
       </c>
-      <c r="F13" s="48">
+      <c r="F13" s="44">
         <f t="shared" si="4"/>
         <v>0.70794578438413791</v>
       </c>
-      <c r="G13" s="51">
+      <c r="G13" s="47">
         <f>ABS(E13)</f>
         <v>1.5</v>
       </c>
@@ -1379,7 +1423,7 @@
         <f t="shared" si="1"/>
         <v>-25</v>
       </c>
-      <c r="R13" s="60">
+      <c r="R13" s="56">
         <f t="shared" si="3"/>
         <v>3.1622776601683769</v>
       </c>
@@ -1392,18 +1436,18 @@
       <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="50" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="25">
         <v>14</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="39">
         <f t="shared" si="4"/>
         <v>25.118864315095799</v>
       </c>
-      <c r="G14" s="51">
+      <c r="G14" s="47">
         <v>1.4</v>
       </c>
       <c r="H14" s="14">
@@ -1430,11 +1474,11 @@
       <c r="O14">
         <v>21</v>
       </c>
-      <c r="Q14" s="58">
+      <c r="Q14" s="54">
         <f t="shared" si="1"/>
         <v>-26.5</v>
       </c>
-      <c r="R14" s="60">
+      <c r="R14" s="56">
         <f t="shared" si="3"/>
         <v>2.2387211385683328</v>
       </c>
@@ -1460,11 +1504,11 @@
       <c r="E15" s="13">
         <v>-2</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="39">
         <f t="shared" si="4"/>
         <v>0.63095734448019325</v>
       </c>
-      <c r="G15" s="51">
+      <c r="G15" s="47">
         <f>ABS(E15)</f>
         <v>2</v>
       </c>
@@ -1493,7 +1537,7 @@
         <f t="shared" si="1"/>
         <v>-12.5</v>
       </c>
-      <c r="R15" s="60">
+      <c r="R15" s="56">
         <f t="shared" si="3"/>
         <v>56.234132519034887</v>
       </c>
@@ -1503,10 +1547,10 @@
       </c>
     </row>
     <row r="16" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="50" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="7"/>
@@ -1517,7 +1561,7 @@
         <f t="shared" si="4"/>
         <v>0.19952623149688795</v>
       </c>
-      <c r="G16" s="52">
+      <c r="G16" s="48">
         <v>7</v>
       </c>
       <c r="H16" s="17">
@@ -1548,11 +1592,11 @@
       <c r="P16" s="7">
         <v>-10</v>
       </c>
-      <c r="Q16" s="58">
+      <c r="Q16" s="54">
         <f t="shared" si="1"/>
         <v>-14.5</v>
       </c>
-      <c r="R16" s="61">
+      <c r="R16" s="57">
         <f t="shared" si="3"/>
         <v>35.481338923357477</v>
       </c>
@@ -1568,7 +1612,7 @@
         <f t="shared" si="8"/>
         <v>3.23634126004817E-2</v>
       </c>
-      <c r="W16" s="55" t="s">
+      <c r="W16" s="51" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1582,11 +1626,11 @@
       <c r="E17" s="13">
         <v>-1.4</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="39">
         <f t="shared" si="4"/>
         <v>0.72443596007499012</v>
       </c>
-      <c r="G17" s="51">
+      <c r="G17" s="47">
         <f>ABS(E17)</f>
         <v>1.4</v>
       </c>
@@ -1615,7 +1659,7 @@
         <f t="shared" si="1"/>
         <v>-21.5</v>
       </c>
-      <c r="R17" s="60">
+      <c r="R17" s="56">
         <f t="shared" si="3"/>
         <v>7.0794578438413627</v>
       </c>
@@ -1628,18 +1672,18 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="42">
+      <c r="D18" s="37"/>
+      <c r="E18" s="38">
         <v>16</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="39">
         <f t="shared" si="4"/>
         <v>39.810717055349755</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="49">
         <v>7</v>
       </c>
       <c r="H18" s="24">
@@ -1669,11 +1713,11 @@
       <c r="P18">
         <v>-7</v>
       </c>
-      <c r="Q18" s="58">
+      <c r="Q18" s="54">
         <f t="shared" si="1"/>
         <v>-22.9</v>
       </c>
-      <c r="R18" s="60">
+      <c r="R18" s="56">
         <f t="shared" si="3"/>
         <v>5.1286138399136441</v>
       </c>
@@ -1689,7 +1733,7 @@
       <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="27">
         <f>-0.5-6.3-0.8</f>
         <v>-7.6</v>
       </c>
@@ -1697,7 +1741,7 @@
         <f t="shared" si="4"/>
         <v>0.17378008287493749</v>
       </c>
-      <c r="G19" s="51">
+      <c r="G19" s="47">
         <f>ABS(E19)</f>
         <v>7.6</v>
       </c>
@@ -1726,7 +1770,7 @@
         <f>Q20-E19</f>
         <v>-6.9</v>
       </c>
-      <c r="R19" s="60">
+      <c r="R19" s="56">
         <f t="shared" si="3"/>
         <v>204.17379446695287</v>
       </c>
@@ -1736,21 +1780,21 @@
       </c>
     </row>
     <row r="20" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="50" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="15">
         <v>-1.5</v>
       </c>
-      <c r="F20" s="48">
+      <c r="F20" s="44">
         <f t="shared" si="4"/>
         <v>0.70794578438413791</v>
       </c>
-      <c r="G20" s="51">
+      <c r="G20" s="47">
         <f>ABS(E20)</f>
         <v>1.5</v>
       </c>
@@ -1779,7 +1823,7 @@
         <f t="shared" ref="Q20:Q21" si="20">Q21-E20</f>
         <v>-14.5</v>
       </c>
-      <c r="R20" s="60">
+      <c r="R20" s="56">
         <f t="shared" si="3"/>
         <v>35.481338923357477</v>
       </c>
@@ -1789,18 +1833,18 @@
       </c>
     </row>
     <row r="21" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="30"/>
-      <c r="C21" s="39" t="s">
+      <c r="B21" s="59"/>
+      <c r="C21" s="35" t="s">
         <v>46</v>
       </c>
       <c r="E21" s="26">
         <v>26</v>
       </c>
-      <c r="F21" s="49">
+      <c r="F21" s="45">
         <f t="shared" si="4"/>
         <v>398.10717055349761</v>
       </c>
-      <c r="G21" s="53">
+      <c r="G21" s="49">
         <v>8</v>
       </c>
       <c r="H21" s="24">
@@ -1830,11 +1874,11 @@
       <c r="P21">
         <v>-17</v>
       </c>
-      <c r="Q21" s="58">
+      <c r="Q21" s="54">
         <f t="shared" si="20"/>
         <v>-16</v>
       </c>
-      <c r="R21" s="60">
+      <c r="R21" s="56">
         <f t="shared" si="3"/>
         <v>25.118864315095792</v>
       </c>
@@ -1853,18 +1897,18 @@
       <c r="E22" s="13">
         <v>0</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="39">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G22" s="51">
+      <c r="G22" s="47">
         <v>27</v>
       </c>
       <c r="H22" s="14">
         <f t="shared" si="2"/>
         <v>501.18723362727269</v>
       </c>
-      <c r="J22" s="43">
+      <c r="J22" s="39">
         <f t="shared" si="17"/>
         <v>1.4922408497981681</v>
       </c>
@@ -1901,7 +1945,7 @@
     </row>
     <row r="23" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E23" s="18"/>
-      <c r="F23" s="50"/>
+      <c r="F23" s="46"/>
       <c r="G23" s="18"/>
       <c r="H23" s="19"/>
       <c r="J23" s="1"/>
@@ -1913,24 +1957,24 @@
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.25">
       <c r="N24" s="2"/>
-      <c r="AB24" s="29" t="s">
+      <c r="AB24" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="AC24" s="29"/>
-      <c r="AD24" s="29"/>
-      <c r="AE24" s="29"/>
-      <c r="AF24" s="29"/>
-      <c r="AG24" s="29"/>
+      <c r="AC24" s="62"/>
+      <c r="AD24" s="62"/>
+      <c r="AE24" s="62"/>
+      <c r="AF24" s="62"/>
+      <c r="AG24" s="62"/>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="AB25" s="28" t="s">
+      <c r="AB25" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="28"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-      <c r="AG25" s="28"/>
+      <c r="AC25" s="61"/>
+      <c r="AD25" s="61"/>
+      <c r="AE25" s="61"/>
+      <c r="AF25" s="61"/>
+      <c r="AG25" s="61"/>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AB26">
@@ -1953,7 +1997,7 @@
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z27" s="27" t="s">
+      <c r="Z27" s="60" t="s">
         <v>23</v>
       </c>
       <c r="AA27" s="6">
@@ -1979,7 +2023,7 @@
       </c>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z28" s="27"/>
+      <c r="Z28" s="60"/>
       <c r="AA28" s="6">
         <v>-10</v>
       </c>
@@ -2003,7 +2047,7 @@
       </c>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z29" s="27"/>
+      <c r="Z29" s="60"/>
       <c r="AA29" s="6">
         <v>-12</v>
       </c>
@@ -2029,7 +2073,7 @@
     <row r="30" spans="2:33" x14ac:dyDescent="0.25">
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="Z30" s="27"/>
+      <c r="Z30" s="60"/>
       <c r="AA30" s="6">
         <v>-14</v>
       </c>
@@ -2053,7 +2097,7 @@
       </c>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z31" s="27"/>
+      <c r="Z31" s="60"/>
       <c r="AA31" s="6">
         <v>-16</v>
       </c>
@@ -2077,7 +2121,7 @@
       </c>
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z32" s="27"/>
+      <c r="Z32" s="60"/>
       <c r="AA32" s="6">
         <v>-18</v>
       </c>
@@ -2105,25 +2149,25 @@
     </row>
     <row r="34" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z34" s="6"/>
-      <c r="AB34" s="29" t="s">
+      <c r="AB34" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="AC34" s="29"/>
-      <c r="AD34" s="29"/>
-      <c r="AE34" s="29"/>
-      <c r="AF34" s="29"/>
-      <c r="AG34" s="29"/>
+      <c r="AC34" s="62"/>
+      <c r="AD34" s="62"/>
+      <c r="AE34" s="62"/>
+      <c r="AF34" s="62"/>
+      <c r="AG34" s="62"/>
     </row>
     <row r="35" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z35" s="6"/>
-      <c r="AB35" s="28" t="s">
+      <c r="AB35" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="AC35" s="28"/>
-      <c r="AD35" s="28"/>
-      <c r="AE35" s="28"/>
-      <c r="AF35" s="28"/>
-      <c r="AG35" s="28"/>
+      <c r="AC35" s="61"/>
+      <c r="AD35" s="61"/>
+      <c r="AE35" s="61"/>
+      <c r="AF35" s="61"/>
+      <c r="AG35" s="61"/>
     </row>
     <row r="36" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z36" s="6"/>
@@ -2147,7 +2191,7 @@
       </c>
     </row>
     <row r="37" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z37" s="27" t="s">
+      <c r="Z37" s="60" t="s">
         <v>23</v>
       </c>
       <c r="AA37" s="6">
@@ -2173,7 +2217,7 @@
       </c>
     </row>
     <row r="38" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z38" s="27"/>
+      <c r="Z38" s="60"/>
       <c r="AA38" s="6">
         <v>-10</v>
       </c>
@@ -2197,7 +2241,7 @@
       </c>
     </row>
     <row r="39" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z39" s="27"/>
+      <c r="Z39" s="60"/>
       <c r="AA39" s="6">
         <v>-12</v>
       </c>
@@ -2221,7 +2265,7 @@
       </c>
     </row>
     <row r="40" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z40" s="27"/>
+      <c r="Z40" s="60"/>
       <c r="AA40" s="6">
         <v>-14</v>
       </c>
@@ -2245,7 +2289,7 @@
       </c>
     </row>
     <row r="41" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z41" s="27"/>
+      <c r="Z41" s="60"/>
       <c r="AA41" s="6">
         <v>-16</v>
       </c>
@@ -2269,7 +2313,7 @@
       </c>
     </row>
     <row r="42" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z42" s="27"/>
+      <c r="Z42" s="60"/>
       <c r="AA42" s="6">
         <v>-18</v>
       </c>
@@ -2297,25 +2341,25 @@
     </row>
     <row r="44" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z44" s="6"/>
-      <c r="AB44" s="29" t="s">
+      <c r="AB44" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="29"/>
-      <c r="AF44" s="29"/>
-      <c r="AG44" s="29"/>
+      <c r="AC44" s="62"/>
+      <c r="AD44" s="62"/>
+      <c r="AE44" s="62"/>
+      <c r="AF44" s="62"/>
+      <c r="AG44" s="62"/>
     </row>
     <row r="45" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z45" s="6"/>
-      <c r="AB45" s="28" t="s">
+      <c r="AB45" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="AC45" s="28"/>
-      <c r="AD45" s="28"/>
-      <c r="AE45" s="28"/>
-      <c r="AF45" s="28"/>
-      <c r="AG45" s="28"/>
+      <c r="AC45" s="61"/>
+      <c r="AD45" s="61"/>
+      <c r="AE45" s="61"/>
+      <c r="AF45" s="61"/>
+      <c r="AG45" s="61"/>
     </row>
     <row r="46" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z46" s="6"/>
@@ -2339,7 +2383,7 @@
       </c>
     </row>
     <row r="47" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z47" s="27" t="s">
+      <c r="Z47" s="60" t="s">
         <v>23</v>
       </c>
       <c r="AA47" s="6">
@@ -2365,7 +2409,7 @@
       </c>
     </row>
     <row r="48" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z48" s="27"/>
+      <c r="Z48" s="60"/>
       <c r="AA48" s="6">
         <v>-10</v>
       </c>
@@ -2389,7 +2433,7 @@
       </c>
     </row>
     <row r="49" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z49" s="27"/>
+      <c r="Z49" s="60"/>
       <c r="AA49" s="6">
         <v>-12</v>
       </c>
@@ -2413,7 +2457,7 @@
       </c>
     </row>
     <row r="50" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z50" s="27"/>
+      <c r="Z50" s="60"/>
       <c r="AA50" s="6">
         <v>-14</v>
       </c>
@@ -2437,7 +2481,7 @@
       </c>
     </row>
     <row r="51" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z51" s="27"/>
+      <c r="Z51" s="60"/>
       <c r="AA51" s="6">
         <v>-16</v>
       </c>
@@ -2461,7 +2505,7 @@
       </c>
     </row>
     <row r="52" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z52" s="27"/>
+      <c r="Z52" s="60"/>
       <c r="AA52" s="6">
         <v>-18</v>
       </c>
@@ -2655,4 +2699,150 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E9:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G9" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="66"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="67"/>
+      <c r="I10" s="66"/>
+    </row>
+    <row r="11" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="65">
+        <v>1</v>
+      </c>
+      <c r="G11" s="65">
+        <v>1</v>
+      </c>
+      <c r="H11" s="65">
+        <v>1</v>
+      </c>
+      <c r="I11" s="64"/>
+    </row>
+    <row r="12" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="64">
+        <v>-7</v>
+      </c>
+      <c r="G12" s="64">
+        <v>-7</v>
+      </c>
+      <c r="H12" s="64">
+        <v>-7</v>
+      </c>
+      <c r="I12" s="64"/>
+    </row>
+    <row r="13" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>-2</v>
+      </c>
+      <c r="G13">
+        <v>-2</v>
+      </c>
+      <c r="H13">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="14" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14">
+        <v>15.6</v>
+      </c>
+      <c r="G14">
+        <v>24</v>
+      </c>
+      <c r="H14">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="15" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <v>-2</v>
+      </c>
+      <c r="G15">
+        <v>-2</v>
+      </c>
+      <c r="H15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16">
+        <v>15.6</v>
+      </c>
+      <c r="G16">
+        <v>15.6</v>
+      </c>
+      <c r="H16">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="63">
+        <f>SUM(F11:F18)</f>
+        <v>36.799999999999997</v>
+      </c>
+      <c r="G19" s="63">
+        <f>SUM(G11:G18)</f>
+        <v>29.6</v>
+      </c>
+      <c r="H19" s="63">
+        <f>SUM(H11:H18)</f>
+        <v>21.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
* further detailing graviton_master spreadsheet
</commit_message>
<xml_diff>
--- a/docs/graviton_master.xlsx
+++ b/docs/graviton_master.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17055" windowHeight="12030" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17055" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="rx_chain" sheetId="1" r:id="rId1"/>
-    <sheet name="tx_chain" sheetId="2" r:id="rId2"/>
+    <sheet name="phase_noise" sheetId="4" r:id="rId2"/>
+    <sheet name="tx_chain" sheetId="2" r:id="rId3"/>
+    <sheet name="power_budget" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t xml:space="preserve">Graviton Receiver Analog Front End Cascade Analysis </t>
   </si>
@@ -211,6 +213,30 @@
   </si>
   <si>
     <t>proposed</t>
+  </si>
+  <si>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>Imax</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>Vmin</t>
+  </si>
+  <si>
+    <t>Vmax</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>PP5V</t>
+  </si>
+  <si>
+    <t>VIN48V</t>
   </si>
 </sst>
 </file>
@@ -927,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AG52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,11 +1134,11 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="53">
         <f t="shared" ref="Q7:Q18" si="1">Q8-E7</f>
-        <v>-40.4</v>
+        <v>-31.4</v>
       </c>
       <c r="R7" s="55">
         <f>10^((Q7-30)/10)*1000000</f>
-        <v>9.1201083935590621E-2</v>
+        <v>0.72443596007499</v>
       </c>
     </row>
     <row r="8" spans="2:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1127,6 +1153,7 @@
         <v>0.79432823472428149</v>
       </c>
       <c r="G8" s="47">
+        <f>ABS(E8)</f>
         <v>1</v>
       </c>
       <c r="H8" s="14">
@@ -1152,11 +1179,11 @@
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="1"/>
-        <v>-40.4</v>
+        <v>-31.4</v>
       </c>
       <c r="R8" s="56">
         <f t="shared" ref="R8:R22" si="3">10^((Q8-30)/10)*1000000</f>
-        <v>9.1201083935590621E-2</v>
+        <v>0.72443596007499</v>
       </c>
       <c r="V8" s="3">
         <f>K8-K7</f>
@@ -1201,11 +1228,11 @@
       </c>
       <c r="Q9" s="2">
         <f t="shared" si="1"/>
-        <v>-41.4</v>
+        <v>-32.4</v>
       </c>
       <c r="R9" s="56">
         <f t="shared" si="3"/>
-        <v>7.2443596007498792E-2</v>
+        <v>0.57543993733715548</v>
       </c>
       <c r="V9" s="3">
         <f t="shared" ref="V9:V22" si="8">K9-K8</f>
@@ -1250,11 +1277,11 @@
       </c>
       <c r="Q10" s="2">
         <f t="shared" si="1"/>
-        <v>-41.4</v>
+        <v>-32.4</v>
       </c>
       <c r="R10" s="56">
         <f t="shared" si="3"/>
-        <v>7.2443596007498792E-2</v>
+        <v>0.57543993733715548</v>
       </c>
       <c r="V10" s="3">
         <f t="shared" si="8"/>
@@ -1308,18 +1335,18 @@
       </c>
       <c r="Q11" s="54">
         <f>Q12-E11</f>
-        <v>-41.4</v>
+        <v>-32.4</v>
       </c>
       <c r="R11" s="56">
         <f t="shared" si="3"/>
-        <v>7.2443596007498792E-2</v>
+        <v>0.57543993733715548</v>
       </c>
       <c r="T11">
         <v>19.100000000000001</v>
       </c>
       <c r="U11">
         <f>Q11 - (T11-Q11)*3</f>
-        <v>-222.9</v>
+        <v>-186.9</v>
       </c>
       <c r="V11" s="3">
         <f t="shared" si="8"/>
@@ -1368,11 +1395,11 @@
       </c>
       <c r="Q12" s="2">
         <f t="shared" ref="Q12" si="14">Q13-E12</f>
-        <v>-23</v>
+        <v>-14</v>
       </c>
       <c r="R12" s="56">
         <f t="shared" ref="R12" si="15">10^((Q12-30)/10)*1000000</f>
-        <v>5.0118723362727193</v>
+        <v>39.810717055349635</v>
       </c>
       <c r="V12" s="3">
         <f t="shared" si="8"/>
@@ -1388,48 +1415,48 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="15">
-        <v>-1.5</v>
+        <v>-8</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="4"/>
-        <v>0.70794578438413791</v>
+        <v>0.15848931924611132</v>
       </c>
       <c r="G13" s="47">
         <f>ABS(E13)</f>
-        <v>1.5</v>
+        <v>8</v>
       </c>
       <c r="H13" s="14">
         <f t="shared" si="2"/>
-        <v>1.4125375446227544</v>
+        <v>6.3095734448019343</v>
       </c>
       <c r="J13" s="2">
         <f>J12+((H13-1)/N12)</f>
-        <v>1.3622177066202468</v>
+        <v>1.5034497647008338</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="0"/>
-        <v>1.3424652110698347</v>
+        <v>1.770889214437138</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13">
         <f>E13+M12</f>
-        <v>13.899999999999999</v>
+        <v>7.3999999999999986</v>
       </c>
       <c r="N13" s="2">
         <f>N12*F13</f>
-        <v>24.547089156850305</v>
+        <v>5.4954087385762449</v>
       </c>
       <c r="Q13" s="2">
         <f t="shared" si="1"/>
-        <v>-25</v>
+        <v>-16</v>
       </c>
       <c r="R13" s="56">
         <f t="shared" si="3"/>
-        <v>3.1622776601683769</v>
+        <v>25.118864315095792</v>
       </c>
       <c r="V13" s="3">
         <f>K13-K12</f>
-        <v>3.8098229048106891E-2</v>
+        <v>0.46652223241541013</v>
       </c>
     </row>
     <row r="14" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1456,42 +1483,42 @@
       </c>
       <c r="J14" s="2">
         <f t="shared" si="5"/>
-        <v>1.3777138113588705</v>
+        <v>1.5726683219907935</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="0"/>
-        <v>1.3915901216089965</v>
+        <v>1.9663713895014889</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14">
         <f t="shared" si="6"/>
-        <v>27.9</v>
+        <v>21.4</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" si="7"/>
-        <v>616.59500186148216</v>
+        <v>138.03842646028846</v>
       </c>
       <c r="O14">
         <v>21</v>
       </c>
       <c r="Q14" s="54">
         <f t="shared" si="1"/>
-        <v>-26.5</v>
+        <v>-24</v>
       </c>
       <c r="R14" s="56">
         <f t="shared" si="3"/>
-        <v>2.2387211385683328</v>
+        <v>3.9810717055349656</v>
       </c>
       <c r="T14">
         <v>21</v>
       </c>
       <c r="U14">
         <f>Q14 - (T14-Q14)*3</f>
-        <v>-169</v>
+        <v>-159</v>
       </c>
       <c r="V14" s="3">
         <f t="shared" si="8"/>
-        <v>4.9124910539161792E-2</v>
+        <v>0.19548217506435095</v>
       </c>
     </row>
     <row r="15" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1518,32 +1545,32 @@
       </c>
       <c r="J15" s="2">
         <f t="shared" si="5"/>
-        <v>1.3786623970442804</v>
+        <v>1.5769054986050124</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="0"/>
-        <v>1.3945793038823999</v>
+        <v>1.9780566754315518</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15">
         <f t="shared" si="6"/>
-        <v>25.9</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="7"/>
-        <v>389.04514499428058</v>
+        <v>87.096358995608057</v>
       </c>
       <c r="Q15" s="2">
         <f t="shared" si="1"/>
-        <v>-12.5</v>
+        <v>-10</v>
       </c>
       <c r="R15" s="56">
         <f t="shared" si="3"/>
-        <v>56.234132519034887</v>
+        <v>100</v>
       </c>
       <c r="V15" s="3">
         <f t="shared" si="8"/>
-        <v>2.9891822734033902E-3</v>
+        <v>1.1685285930062905E-2</v>
       </c>
     </row>
     <row r="16" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1571,20 +1598,20 @@
       <c r="I16" s="7"/>
       <c r="J16" s="10">
         <f t="shared" si="5"/>
-        <v>1.388974496778443</v>
+        <v>1.6229679561237593</v>
       </c>
       <c r="K16" s="10">
         <f t="shared" si="0"/>
-        <v>1.4269427164828816</v>
+        <v>2.1030994520145514</v>
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="7">
         <f t="shared" si="6"/>
-        <v>18.899999999999999</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="N16" s="10">
         <f t="shared" si="7"/>
-        <v>77.62471166286916</v>
+        <v>17.378008287493753</v>
       </c>
       <c r="O16" s="7">
         <v>0</v>
@@ -1594,11 +1621,11 @@
       </c>
       <c r="Q16" s="54">
         <f t="shared" si="1"/>
-        <v>-14.5</v>
+        <v>-12</v>
       </c>
       <c r="R16" s="57">
         <f t="shared" si="3"/>
-        <v>35.481338923357477</v>
+        <v>63.095734448019279</v>
       </c>
       <c r="S16" s="7"/>
       <c r="T16" s="7">
@@ -1606,11 +1633,11 @@
       </c>
       <c r="U16" s="7">
         <f>Q16 - (T16-Q16)*3</f>
-        <v>-166</v>
+        <v>-156</v>
       </c>
       <c r="V16" s="8">
         <f t="shared" si="8"/>
-        <v>3.23634126004817E-2</v>
+        <v>0.12504277658299956</v>
       </c>
       <c r="W16" s="51" t="s">
         <v>12</v>
@@ -1640,32 +1667,32 @@
       </c>
       <c r="J17" s="2">
         <f t="shared" si="5"/>
-        <v>1.3938747953619008</v>
+        <v>1.6448567858624719</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="0"/>
-        <v>1.4422376506363574</v>
+        <v>2.1612809084692648</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17">
         <f t="shared" ref="M17:M19" si="16">E17+M16</f>
-        <v>17.5</v>
+        <v>10.999999999999998</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="7"/>
-        <v>56.234132519034901</v>
+        <v>12.589254117941671</v>
       </c>
       <c r="Q17" s="2">
         <f t="shared" si="1"/>
-        <v>-21.5</v>
+        <v>-19</v>
       </c>
       <c r="R17" s="56">
         <f t="shared" si="3"/>
-        <v>7.0794578438413627</v>
+        <v>12.589254117941659</v>
       </c>
       <c r="V17" s="3">
         <f t="shared" si="8"/>
-        <v>1.5294934153475825E-2</v>
+        <v>5.8181456454713398E-2</v>
       </c>
     </row>
     <row r="18" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1692,20 +1719,20 @@
       </c>
       <c r="J18" s="2">
         <f t="shared" si="5"/>
-        <v>1.4652170950748862</v>
+        <v>1.963531132943541</v>
       </c>
       <c r="K18" s="20">
         <f t="shared" si="0"/>
-        <v>1.6590197705050622</v>
+        <v>2.9303779165603934</v>
       </c>
       <c r="L18" s="20"/>
       <c r="M18">
         <f t="shared" si="16"/>
-        <v>33.5</v>
+        <v>27</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="7"/>
-        <v>2238.7211385683408</v>
+        <v>501.18723362727263</v>
       </c>
       <c r="O18">
         <v>-6</v>
@@ -1715,15 +1742,15 @@
       </c>
       <c r="Q18" s="54">
         <f t="shared" si="1"/>
-        <v>-22.9</v>
+        <v>-20.399999999999999</v>
       </c>
       <c r="R18" s="56">
         <f t="shared" si="3"/>
-        <v>5.1286138399136441</v>
+        <v>9.1201083935590823</v>
       </c>
       <c r="V18" s="3">
         <f t="shared" si="8"/>
-        <v>0.21678211986870477</v>
+        <v>0.76909700809112858</v>
       </c>
     </row>
     <row r="19" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1751,32 +1778,32 @@
       </c>
       <c r="J19" s="2">
         <f t="shared" si="5"/>
-        <v>1.4673408072655041</v>
+        <v>1.9730174068435409</v>
       </c>
       <c r="K19" s="20">
         <f t="shared" si="0"/>
-        <v>1.6653099559164675</v>
+        <v>2.9513091680959085</v>
       </c>
       <c r="L19" s="20"/>
       <c r="M19">
         <f t="shared" si="16"/>
-        <v>25.9</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="7"/>
-        <v>389.04514499428069</v>
+        <v>87.096358995608099</v>
       </c>
       <c r="Q19" s="2">
         <f>Q20-E19</f>
-        <v>-6.9</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="R19" s="56">
         <f t="shared" si="3"/>
-        <v>204.17379446695287</v>
+        <v>363.07805477010101</v>
       </c>
       <c r="V19" s="3">
         <f t="shared" si="8"/>
-        <v>6.2901854114052469E-3</v>
+        <v>2.0931251535515116E-2</v>
       </c>
     </row>
     <row r="20" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1788,48 +1815,48 @@
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="15">
-        <v>-1.5</v>
+        <v>-4</v>
       </c>
       <c r="F20" s="44">
         <f t="shared" si="4"/>
-        <v>0.70794578438413791</v>
+        <v>0.3981071705534972</v>
       </c>
       <c r="G20" s="47">
         <f>ABS(E20)</f>
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="H20" s="14">
         <f t="shared" si="2"/>
-        <v>1.4125375446227544</v>
+        <v>2.5118864315095806</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20:J22" si="17">J19+((H20-1)/N19)</f>
-        <v>1.4684011920304363</v>
+        <v>1.9903761856598381</v>
       </c>
       <c r="K20" s="20">
         <f t="shared" si="0"/>
-        <v>1.6684472838713211</v>
+        <v>2.9893516681981103</v>
       </c>
       <c r="L20" s="20"/>
       <c r="M20">
         <f t="shared" ref="M20:M22" si="18">E20+M19</f>
-        <v>24.4</v>
+        <v>15.399999999999999</v>
       </c>
       <c r="N20" s="2">
         <f t="shared" ref="N20:N22" si="19">N19*F20</f>
-        <v>275.42287033381672</v>
+        <v>34.673685045253173</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20:Q21" si="20">Q21-E20</f>
-        <v>-14.5</v>
+        <v>-12</v>
       </c>
       <c r="R20" s="56">
         <f t="shared" si="3"/>
-        <v>35.481338923357477</v>
+        <v>63.095734448019279</v>
       </c>
       <c r="V20" s="3">
         <f t="shared" si="8"/>
-        <v>3.1373279548536637E-3</v>
+        <v>3.8042500102201782E-2</v>
       </c>
     </row>
     <row r="21" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1853,20 +1880,20 @@
       </c>
       <c r="J21" s="2">
         <f t="shared" si="17"/>
-        <v>1.4876790880104129</v>
+        <v>2.1435059564895704</v>
       </c>
       <c r="K21" s="21">
         <f t="shared" si="0"/>
-        <v>1.7250925826820693</v>
+        <v>3.31124694689179</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21">
         <f t="shared" si="18"/>
-        <v>50.4</v>
+        <v>41.4</v>
       </c>
       <c r="N21" s="2">
         <f t="shared" si="19"/>
-        <v>109647.81961431864</v>
+        <v>13803.842646028865</v>
       </c>
       <c r="O21">
         <v>-16</v>
@@ -1884,7 +1911,7 @@
       </c>
       <c r="V21" s="3">
         <f t="shared" si="8"/>
-        <v>5.6645298810748201E-2</v>
+        <v>0.32189527869367973</v>
       </c>
     </row>
     <row r="22" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1910,20 +1937,20 @@
       </c>
       <c r="J22" s="39">
         <f t="shared" si="17"/>
-        <v>1.4922408497981681</v>
+        <v>2.1797413183705729</v>
       </c>
       <c r="K22" s="22">
         <f t="shared" si="0"/>
-        <v>1.738389245418674</v>
+        <v>3.38404956599926</v>
       </c>
       <c r="L22" s="20"/>
       <c r="M22">
         <f t="shared" si="18"/>
-        <v>50.4</v>
+        <v>41.4</v>
       </c>
       <c r="N22" s="2">
         <f t="shared" si="19"/>
-        <v>109647.81961431864</v>
+        <v>13803.842646028865</v>
       </c>
       <c r="O22">
         <v>10</v>
@@ -1940,7 +1967,7 @@
       </c>
       <c r="V22" s="3">
         <f t="shared" si="8"/>
-        <v>1.3296662736604681E-2</v>
+        <v>7.280261910746999E-2</v>
       </c>
     </row>
     <row r="23" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2703,9 +2730,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G9:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="9" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10">
+        <f>4.98*0.98</f>
+        <v>4.8804000000000007</v>
+      </c>
+      <c r="K10">
+        <f>4.98*1.02</f>
+        <v>5.0796000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E9:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
@@ -2845,4 +2923,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more issues tackled. see github for details.
</commit_message>
<xml_diff>
--- a/docs/graviton_master.xlsx
+++ b/docs/graviton_master.xlsx
@@ -648,6 +648,16 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -659,16 +669,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -954,7 +954,7 @@
   <dimension ref="B2:AG52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,7 +1807,7 @@
       </c>
     </row>
     <row r="20" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="65" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="50" t="s">
@@ -1860,7 +1860,7 @@
       </c>
     </row>
     <row r="21" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="59"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="35" t="s">
         <v>46</v>
       </c>
@@ -1984,24 +1984,24 @@
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.25">
       <c r="N24" s="2"/>
-      <c r="AB24" s="62" t="s">
+      <c r="AB24" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AC24" s="62"/>
-      <c r="AD24" s="62"/>
-      <c r="AE24" s="62"/>
-      <c r="AF24" s="62"/>
-      <c r="AG24" s="62"/>
+      <c r="AC24" s="68"/>
+      <c r="AD24" s="68"/>
+      <c r="AE24" s="68"/>
+      <c r="AF24" s="68"/>
+      <c r="AG24" s="68"/>
     </row>
     <row r="25" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="AB25" s="61" t="s">
+      <c r="AB25" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="AC25" s="61"/>
-      <c r="AD25" s="61"/>
-      <c r="AE25" s="61"/>
-      <c r="AF25" s="61"/>
-      <c r="AG25" s="61"/>
+      <c r="AC25" s="67"/>
+      <c r="AD25" s="67"/>
+      <c r="AE25" s="67"/>
+      <c r="AF25" s="67"/>
+      <c r="AG25" s="67"/>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AB26">
@@ -2024,7 +2024,7 @@
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z27" s="60" t="s">
+      <c r="Z27" s="66" t="s">
         <v>23</v>
       </c>
       <c r="AA27" s="6">
@@ -2050,7 +2050,7 @@
       </c>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z28" s="60"/>
+      <c r="Z28" s="66"/>
       <c r="AA28" s="6">
         <v>-10</v>
       </c>
@@ -2074,7 +2074,7 @@
       </c>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z29" s="60"/>
+      <c r="Z29" s="66"/>
       <c r="AA29" s="6">
         <v>-12</v>
       </c>
@@ -2100,7 +2100,7 @@
     <row r="30" spans="2:33" x14ac:dyDescent="0.25">
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="Z30" s="60"/>
+      <c r="Z30" s="66"/>
       <c r="AA30" s="6">
         <v>-14</v>
       </c>
@@ -2124,7 +2124,7 @@
       </c>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z31" s="60"/>
+      <c r="Z31" s="66"/>
       <c r="AA31" s="6">
         <v>-16</v>
       </c>
@@ -2148,7 +2148,7 @@
       </c>
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="Z32" s="60"/>
+      <c r="Z32" s="66"/>
       <c r="AA32" s="6">
         <v>-18</v>
       </c>
@@ -2176,25 +2176,25 @@
     </row>
     <row r="34" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z34" s="6"/>
-      <c r="AB34" s="62" t="s">
+      <c r="AB34" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="AC34" s="62"/>
-      <c r="AD34" s="62"/>
-      <c r="AE34" s="62"/>
-      <c r="AF34" s="62"/>
-      <c r="AG34" s="62"/>
+      <c r="AC34" s="68"/>
+      <c r="AD34" s="68"/>
+      <c r="AE34" s="68"/>
+      <c r="AF34" s="68"/>
+      <c r="AG34" s="68"/>
     </row>
     <row r="35" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z35" s="6"/>
-      <c r="AB35" s="61" t="s">
+      <c r="AB35" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="AC35" s="61"/>
-      <c r="AD35" s="61"/>
-      <c r="AE35" s="61"/>
-      <c r="AF35" s="61"/>
-      <c r="AG35" s="61"/>
+      <c r="AC35" s="67"/>
+      <c r="AD35" s="67"/>
+      <c r="AE35" s="67"/>
+      <c r="AF35" s="67"/>
+      <c r="AG35" s="67"/>
     </row>
     <row r="36" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z36" s="6"/>
@@ -2218,7 +2218,7 @@
       </c>
     </row>
     <row r="37" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z37" s="60" t="s">
+      <c r="Z37" s="66" t="s">
         <v>23</v>
       </c>
       <c r="AA37" s="6">
@@ -2244,7 +2244,7 @@
       </c>
     </row>
     <row r="38" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z38" s="60"/>
+      <c r="Z38" s="66"/>
       <c r="AA38" s="6">
         <v>-10</v>
       </c>
@@ -2268,7 +2268,7 @@
       </c>
     </row>
     <row r="39" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z39" s="60"/>
+      <c r="Z39" s="66"/>
       <c r="AA39" s="6">
         <v>-12</v>
       </c>
@@ -2292,7 +2292,7 @@
       </c>
     </row>
     <row r="40" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z40" s="60"/>
+      <c r="Z40" s="66"/>
       <c r="AA40" s="6">
         <v>-14</v>
       </c>
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="41" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z41" s="60"/>
+      <c r="Z41" s="66"/>
       <c r="AA41" s="6">
         <v>-16</v>
       </c>
@@ -2340,7 +2340,7 @@
       </c>
     </row>
     <row r="42" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z42" s="60"/>
+      <c r="Z42" s="66"/>
       <c r="AA42" s="6">
         <v>-18</v>
       </c>
@@ -2368,25 +2368,25 @@
     </row>
     <row r="44" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z44" s="6"/>
-      <c r="AB44" s="62" t="s">
+      <c r="AB44" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="AC44" s="62"/>
-      <c r="AD44" s="62"/>
-      <c r="AE44" s="62"/>
-      <c r="AF44" s="62"/>
-      <c r="AG44" s="62"/>
+      <c r="AC44" s="68"/>
+      <c r="AD44" s="68"/>
+      <c r="AE44" s="68"/>
+      <c r="AF44" s="68"/>
+      <c r="AG44" s="68"/>
     </row>
     <row r="45" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z45" s="6"/>
-      <c r="AB45" s="61" t="s">
+      <c r="AB45" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="AC45" s="61"/>
-      <c r="AD45" s="61"/>
-      <c r="AE45" s="61"/>
-      <c r="AF45" s="61"/>
-      <c r="AG45" s="61"/>
+      <c r="AC45" s="67"/>
+      <c r="AD45" s="67"/>
+      <c r="AE45" s="67"/>
+      <c r="AF45" s="67"/>
+      <c r="AG45" s="67"/>
     </row>
     <row r="46" spans="26:33" x14ac:dyDescent="0.25">
       <c r="Z46" s="6"/>
@@ -2410,7 +2410,7 @@
       </c>
     </row>
     <row r="47" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z47" s="60" t="s">
+      <c r="Z47" s="66" t="s">
         <v>23</v>
       </c>
       <c r="AA47" s="6">
@@ -2436,7 +2436,7 @@
       </c>
     </row>
     <row r="48" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z48" s="60"/>
+      <c r="Z48" s="66"/>
       <c r="AA48" s="6">
         <v>-10</v>
       </c>
@@ -2460,7 +2460,7 @@
       </c>
     </row>
     <row r="49" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z49" s="60"/>
+      <c r="Z49" s="66"/>
       <c r="AA49" s="6">
         <v>-12</v>
       </c>
@@ -2484,7 +2484,7 @@
       </c>
     </row>
     <row r="50" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z50" s="60"/>
+      <c r="Z50" s="66"/>
       <c r="AA50" s="6">
         <v>-14</v>
       </c>
@@ -2508,7 +2508,7 @@
       </c>
     </row>
     <row r="51" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z51" s="60"/>
+      <c r="Z51" s="66"/>
       <c r="AA51" s="6">
         <v>-16</v>
       </c>
@@ -2532,7 +2532,7 @@
       </c>
     </row>
     <row r="52" spans="26:33" x14ac:dyDescent="0.25">
-      <c r="Z52" s="60"/>
+      <c r="Z52" s="66"/>
       <c r="AA52" s="6">
         <v>-18</v>
       </c>
@@ -2801,43 +2801,43 @@
       </c>
     </row>
     <row r="10" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="66"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="67" t="s">
+      <c r="E10" s="62"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="67"/>
-      <c r="I10" s="66"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="62"/>
     </row>
     <row r="11" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="61">
         <v>1</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="61">
         <v>1</v>
       </c>
-      <c r="H11" s="65">
+      <c r="H11" s="61">
         <v>1</v>
       </c>
-      <c r="I11" s="64"/>
+      <c r="I11" s="60"/>
     </row>
     <row r="12" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="64">
+      <c r="F12" s="60">
         <v>-7</v>
       </c>
-      <c r="G12" s="64">
+      <c r="G12" s="60">
         <v>-7</v>
       </c>
-      <c r="H12" s="64">
+      <c r="H12" s="60">
         <v>-7</v>
       </c>
-      <c r="I12" s="64"/>
+      <c r="I12" s="60"/>
     </row>
     <row r="13" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
@@ -2907,15 +2907,15 @@
       <c r="E19" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="63">
+      <c r="F19" s="59">
         <f>SUM(F11:F18)</f>
         <v>36.799999999999997</v>
       </c>
-      <c r="G19" s="63">
+      <c r="G19" s="59">
         <f>SUM(G11:G18)</f>
         <v>29.6</v>
       </c>
-      <c r="H19" s="63">
+      <c r="H19" s="59">
         <f>SUM(H11:H18)</f>
         <v>21.2</v>
       </c>

</xml_diff>

<commit_message>
fixed all open tickets
</commit_message>
<xml_diff>
--- a/docs/graviton_master.xlsx
+++ b/docs/graviton_master.xlsx
@@ -17,7 +17,7 @@
     <sheet name="tx_chain" sheetId="2" r:id="rId3"/>
     <sheet name="power_budget" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterate="1" iterateCount="1000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
   <si>
     <t xml:space="preserve">Graviton Receiver Analog Front End Cascade Analysis </t>
   </si>
@@ -237,6 +237,27 @@
   </si>
   <si>
     <t>VIN48V</t>
+  </si>
+  <si>
+    <t>meas</t>
+  </si>
+  <si>
+    <t>bw</t>
+  </si>
+  <si>
+    <t>noise floor</t>
+  </si>
+  <si>
+    <t>dbm/Hz</t>
+  </si>
+  <si>
+    <t>noise figure</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>mhz</t>
   </si>
 </sst>
 </file>
@@ -572,7 +593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -670,6 +691,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -954,7 +976,7 @@
   <dimension ref="B2:AG52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+      <selection activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,11 +1156,11 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="53">
         <f t="shared" ref="Q7:Q18" si="1">Q8-E7</f>
-        <v>-31.4</v>
+        <v>-42.9</v>
       </c>
       <c r="R7" s="55">
         <f>10^((Q7-30)/10)*1000000</f>
-        <v>0.72443596007499</v>
+        <v>5.1286138399136226E-2</v>
       </c>
     </row>
     <row r="8" spans="2:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1146,48 +1168,48 @@
         <v>48</v>
       </c>
       <c r="E8" s="13">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="43">
         <f>10^(E8/10)</f>
-        <v>0.79432823472428149</v>
+        <v>1</v>
       </c>
       <c r="G8" s="47">
         <f>ABS(E8)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="14">
         <f t="shared" ref="H8:H22" si="2">10^(G8/10)</f>
-        <v>1.2589254117941673</v>
+        <v>1</v>
       </c>
       <c r="J8" s="2">
         <f>J7+((H8-1)/N7)</f>
-        <v>1.2589254117941673</v>
+        <v>1</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="0"/>
-        <v>1.0000000000000002</v>
+        <v>0</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8">
         <f>E8+M7</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="2">
         <f>N7*F8</f>
-        <v>0.79432823472428149</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="1"/>
-        <v>-31.4</v>
+        <v>-42.9</v>
       </c>
       <c r="R8" s="56">
         <f t="shared" ref="R8:R22" si="3">10^((Q8-30)/10)*1000000</f>
-        <v>0.72443596007499</v>
+        <v>5.1286138399136226E-2</v>
       </c>
       <c r="V8" s="3">
         <f>K8-K7</f>
-        <v>1.0000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
@@ -1211,28 +1233,28 @@
       </c>
       <c r="J9" s="2">
         <f t="shared" ref="J9:J19" si="5">J8+((H9-1)/N8)</f>
-        <v>1.2589254117941673</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="0"/>
-        <v>1.0000000000000002</v>
+        <v>0</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9">
         <f t="shared" ref="M9:M16" si="6">E9+M8</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" ref="N9:N19" si="7">N8*F9</f>
-        <v>0.79432823472428149</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="2">
         <f t="shared" si="1"/>
-        <v>-32.4</v>
+        <v>-42.9</v>
       </c>
       <c r="R9" s="56">
         <f t="shared" si="3"/>
-        <v>0.57543993733715548</v>
+        <v>5.1286138399136226E-2</v>
       </c>
       <c r="V9" s="3">
         <f t="shared" ref="V9:V22" si="8">K9-K8</f>
@@ -1260,28 +1282,28 @@
       </c>
       <c r="J10" s="2">
         <f t="shared" si="5"/>
-        <v>1.2589254117941673</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="0"/>
-        <v>1.0000000000000002</v>
+        <v>0</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="2">
         <f t="shared" si="7"/>
-        <v>0.79432823472428149</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="2">
         <f t="shared" si="1"/>
-        <v>-32.4</v>
+        <v>-42.9</v>
       </c>
       <c r="R10" s="56">
         <f t="shared" si="3"/>
-        <v>0.57543993733715548</v>
+        <v>5.1286138399136226E-2</v>
       </c>
       <c r="V10" s="3">
         <f t="shared" si="8"/>
@@ -1312,20 +1334,20 @@
       </c>
       <c r="J11" s="2">
         <f t="shared" si="5"/>
-        <v>1.3396766874259352</v>
+        <v>1.0641430182243161</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="0"/>
-        <v>1.2700000000000002</v>
+        <v>0.2700000000000003</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11">
         <f t="shared" si="6"/>
-        <v>17.399999999999999</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="N11" s="2">
         <f t="shared" si="7"/>
-        <v>54.954087385762463</v>
+        <v>69.183097091893657</v>
       </c>
       <c r="O11">
         <v>2.4</v>
@@ -1335,22 +1357,22 @@
       </c>
       <c r="Q11" s="54">
         <f>Q12-E11</f>
-        <v>-32.4</v>
+        <v>-42.9</v>
       </c>
       <c r="R11" s="56">
         <f t="shared" si="3"/>
-        <v>0.57543993733715548</v>
+        <v>5.1286138399136226E-2</v>
       </c>
       <c r="T11">
         <v>19.100000000000001</v>
       </c>
       <c r="U11">
         <f>Q11 - (T11-Q11)*3</f>
-        <v>-186.9</v>
+        <v>-228.9</v>
       </c>
       <c r="V11" s="3">
         <f t="shared" si="8"/>
-        <v>0.27</v>
+        <v>0.2700000000000003</v>
       </c>
     </row>
     <row r="12" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1378,32 +1400,32 @@
       </c>
       <c r="J12" s="2">
         <f t="shared" ref="J12" si="11">J11+((H12-1)/N11)</f>
-        <v>1.3503199938711015</v>
+        <v>1.0725972970445345</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" si="0"/>
-        <v>1.3043669820217278</v>
+        <v>0.30436698202172757</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12">
         <f t="shared" ref="M12" si="12">E12+M11</f>
-        <v>15.399999999999999</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="N12" s="2">
         <f t="shared" ref="N12" si="13">N11*F12</f>
-        <v>34.673685045253166</v>
+        <v>43.651583224016605</v>
       </c>
       <c r="Q12" s="2">
         <f t="shared" ref="Q12" si="14">Q13-E12</f>
-        <v>-14</v>
+        <v>-24.5</v>
       </c>
       <c r="R12" s="56">
         <f t="shared" ref="R12" si="15">10^((Q12-30)/10)*1000000</f>
-        <v>39.810717055349635</v>
+        <v>3.5481338923357506</v>
       </c>
       <c r="V12" s="3">
         <f t="shared" si="8"/>
-        <v>3.436698202172761E-2</v>
+        <v>3.4366982021727277E-2</v>
       </c>
     </row>
     <row r="13" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1415,48 +1437,48 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="15">
-        <v>-8</v>
+        <v>-1.5</v>
       </c>
       <c r="F13" s="44">
         <f t="shared" si="4"/>
-        <v>0.15848931924611132</v>
+        <v>0.70794578438413791</v>
       </c>
       <c r="G13" s="47">
         <f>ABS(E13)</f>
-        <v>8</v>
+        <v>1.5</v>
       </c>
       <c r="H13" s="14">
         <f t="shared" si="2"/>
-        <v>6.3095734448019343</v>
+        <v>1.4125375446227544</v>
       </c>
       <c r="J13" s="2">
         <f>J12+((H13-1)/N12)</f>
-        <v>1.5034497647008338</v>
+        <v>1.0820479862098196</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="0"/>
-        <v>1.770889214437138</v>
+        <v>0.34246521106983385</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13">
         <f>E13+M12</f>
-        <v>7.3999999999999986</v>
+        <v>14.899999999999999</v>
       </c>
       <c r="N13" s="2">
         <f>N12*F13</f>
-        <v>5.4954087385762449</v>
+        <v>30.902954325135912</v>
       </c>
       <c r="Q13" s="2">
         <f t="shared" si="1"/>
-        <v>-16</v>
+        <v>-26.5</v>
       </c>
       <c r="R13" s="56">
         <f t="shared" si="3"/>
-        <v>25.118864315095792</v>
+        <v>2.2387211385683328</v>
       </c>
       <c r="V13" s="3">
         <f>K13-K12</f>
-        <v>0.46652223241541013</v>
+        <v>3.809822904810628E-2</v>
       </c>
     </row>
     <row r="14" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1483,42 +1505,42 @@
       </c>
       <c r="J14" s="2">
         <f t="shared" si="5"/>
-        <v>1.5726683219907935</v>
+        <v>1.094356979731953</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="0"/>
-        <v>1.9663713895014889</v>
+        <v>0.39159012160899515</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14">
         <f t="shared" si="6"/>
-        <v>21.4</v>
+        <v>28.9</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" si="7"/>
-        <v>138.03842646028846</v>
+        <v>776.24711662869186</v>
       </c>
       <c r="O14">
         <v>21</v>
       </c>
       <c r="Q14" s="54">
         <f t="shared" si="1"/>
-        <v>-24</v>
+        <v>-28</v>
       </c>
       <c r="R14" s="56">
         <f t="shared" si="3"/>
-        <v>3.9810717055349656</v>
+        <v>1.5848931924611112</v>
       </c>
       <c r="T14">
         <v>21</v>
       </c>
       <c r="U14">
         <f>Q14 - (T14-Q14)*3</f>
-        <v>-159</v>
+        <v>-175</v>
       </c>
       <c r="V14" s="3">
         <f t="shared" si="8"/>
-        <v>0.19548217506435095</v>
+        <v>4.9124910539161293E-2</v>
       </c>
     </row>
     <row r="15" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1545,32 +1567,32 @@
       </c>
       <c r="J15" s="2">
         <f t="shared" si="5"/>
-        <v>1.5769054986050124</v>
+        <v>1.0951104681249293</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="0"/>
-        <v>1.9780566754315518</v>
+        <v>0.39457930388239837</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15">
         <f t="shared" si="6"/>
-        <v>19.399999999999999</v>
+        <v>26.9</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="7"/>
-        <v>87.096358995608057</v>
+        <v>489.77881936844625</v>
       </c>
       <c r="Q15" s="2">
         <f t="shared" si="1"/>
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="R15" s="56">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>39.810717055349635</v>
       </c>
       <c r="V15" s="3">
         <f t="shared" si="8"/>
-        <v>1.1685285930062905E-2</v>
+        <v>2.9891822734032236E-3</v>
       </c>
     </row>
     <row r="16" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1598,20 +1620,20 @@
       <c r="I16" s="7"/>
       <c r="J16" s="10">
         <f t="shared" si="5"/>
-        <v>1.6229679561237593</v>
+        <v>1.1033016601030674</v>
       </c>
       <c r="K16" s="10">
         <f t="shared" si="0"/>
-        <v>2.1030994520145514</v>
+        <v>0.42694271648287996</v>
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="7">
         <f t="shared" si="6"/>
-        <v>12.399999999999999</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="N16" s="10">
         <f t="shared" si="7"/>
-        <v>17.378008287493753</v>
+        <v>97.723722095581067</v>
       </c>
       <c r="O16" s="7">
         <v>0</v>
@@ -1621,11 +1643,11 @@
       </c>
       <c r="Q16" s="54">
         <f t="shared" si="1"/>
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="R16" s="57">
         <f t="shared" si="3"/>
-        <v>63.095734448019279</v>
+        <v>25.118864315095792</v>
       </c>
       <c r="S16" s="7"/>
       <c r="T16" s="7">
@@ -1633,11 +1655,11 @@
       </c>
       <c r="U16" s="7">
         <f>Q16 - (T16-Q16)*3</f>
-        <v>-156</v>
+        <v>-172</v>
       </c>
       <c r="V16" s="8">
         <f t="shared" si="8"/>
-        <v>0.12504277658299956</v>
+        <v>3.2363412600481589E-2</v>
       </c>
       <c r="W16" s="51" t="s">
         <v>12</v>
@@ -1667,32 +1689,32 @@
       </c>
       <c r="J17" s="2">
         <f t="shared" si="5"/>
-        <v>1.6448567858624719</v>
+        <v>1.1071941056264873</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="0"/>
-        <v>2.1612809084692648</v>
+        <v>0.44223765063635562</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17">
         <f t="shared" ref="M17:M19" si="16">E17+M16</f>
-        <v>10.999999999999998</v>
+        <v>18.5</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="7"/>
-        <v>12.589254117941671</v>
+        <v>70.794578438413794</v>
       </c>
       <c r="Q17" s="2">
         <f t="shared" si="1"/>
-        <v>-19</v>
+        <v>-23</v>
       </c>
       <c r="R17" s="56">
         <f t="shared" si="3"/>
-        <v>12.589254117941659</v>
+        <v>5.0118723362727193</v>
       </c>
       <c r="V17" s="3">
         <f t="shared" si="8"/>
-        <v>5.8181456454713398E-2</v>
+        <v>1.5294934153475659E-2</v>
       </c>
     </row>
     <row r="18" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1719,20 +1741,20 @@
       </c>
       <c r="J18" s="2">
         <f t="shared" si="5"/>
-        <v>1.963531132943541</v>
+        <v>1.1638633086186736</v>
       </c>
       <c r="K18" s="20">
         <f t="shared" si="0"/>
-        <v>2.9303779165603934</v>
+        <v>0.65901977050506033</v>
       </c>
       <c r="L18" s="20"/>
       <c r="M18">
         <f t="shared" si="16"/>
-        <v>27</v>
+        <v>34.5</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="7"/>
-        <v>501.18723362727263</v>
+        <v>2818.3829312644561</v>
       </c>
       <c r="O18">
         <v>-6</v>
@@ -1742,15 +1764,15 @@
       </c>
       <c r="Q18" s="54">
         <f t="shared" si="1"/>
-        <v>-20.399999999999999</v>
+        <v>-24.4</v>
       </c>
       <c r="R18" s="56">
         <f t="shared" si="3"/>
-        <v>9.1201083935590823</v>
+        <v>3.6307805477010153</v>
       </c>
       <c r="V18" s="3">
         <f t="shared" si="8"/>
-        <v>0.76909700809112858</v>
+        <v>0.21678211986870471</v>
       </c>
     </row>
     <row r="19" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1778,32 +1800,32 @@
       </c>
       <c r="J19" s="2">
         <f t="shared" si="5"/>
-        <v>1.9730174068435409</v>
+        <v>1.1655502331741094</v>
       </c>
       <c r="K19" s="20">
         <f t="shared" si="0"/>
-        <v>2.9513091680959085</v>
+        <v>0.66530995591646536</v>
       </c>
       <c r="L19" s="20"/>
       <c r="M19">
         <f t="shared" si="16"/>
-        <v>19.399999999999999</v>
+        <v>26.9</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="7"/>
-        <v>87.096358995608099</v>
+        <v>489.77881936844642</v>
       </c>
       <c r="Q19" s="2">
         <f>Q20-E19</f>
-        <v>-4.4000000000000004</v>
+        <v>-8.4</v>
       </c>
       <c r="R19" s="56">
         <f t="shared" si="3"/>
-        <v>363.07805477010101</v>
+        <v>144.54397707459268</v>
       </c>
       <c r="V19" s="3">
         <f t="shared" si="8"/>
-        <v>2.0931251535515116E-2</v>
+        <v>6.2901854114050249E-3</v>
       </c>
     </row>
     <row r="20" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1815,48 +1837,48 @@
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="15">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="F20" s="44">
         <f t="shared" si="4"/>
-        <v>0.3981071705534972</v>
+        <v>1</v>
       </c>
       <c r="G20" s="47">
         <f>ABS(E20)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H20" s="14">
         <f t="shared" si="2"/>
-        <v>2.5118864315095806</v>
+        <v>1</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" ref="J20:J22" si="17">J19+((H20-1)/N19)</f>
-        <v>1.9903761856598381</v>
+        <v>1.1655502331741094</v>
       </c>
       <c r="K20" s="20">
         <f t="shared" si="0"/>
-        <v>2.9893516681981103</v>
+        <v>0.66530995591646536</v>
       </c>
       <c r="L20" s="20"/>
       <c r="M20">
         <f t="shared" ref="M20:M22" si="18">E20+M19</f>
-        <v>15.399999999999999</v>
+        <v>26.9</v>
       </c>
       <c r="N20" s="2">
         <f t="shared" ref="N20:N22" si="19">N19*F20</f>
-        <v>34.673685045253173</v>
+        <v>489.77881936844642</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" ref="Q20:Q21" si="20">Q21-E20</f>
-        <v>-12</v>
+        <v>-16</v>
       </c>
       <c r="R20" s="56">
         <f t="shared" si="3"/>
-        <v>63.095734448019279</v>
+        <v>25.118864315095792</v>
       </c>
       <c r="V20" s="3">
         <f t="shared" si="8"/>
-        <v>3.8042500102201782E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1880,20 +1902,20 @@
       </c>
       <c r="J21" s="2">
         <f t="shared" si="17"/>
-        <v>2.1435059564895704</v>
+        <v>1.1763909907463712</v>
       </c>
       <c r="K21" s="21">
         <f t="shared" si="0"/>
-        <v>3.31124694689179</v>
+        <v>0.70551689853971411</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21">
         <f t="shared" si="18"/>
-        <v>41.4</v>
+        <v>52.9</v>
       </c>
       <c r="N21" s="2">
         <f t="shared" si="19"/>
-        <v>13803.842646028865</v>
+        <v>194984.45997580478</v>
       </c>
       <c r="O21">
         <v>-16</v>
@@ -1911,7 +1933,7 @@
       </c>
       <c r="V21" s="3">
         <f t="shared" si="8"/>
-        <v>0.32189527869367973</v>
+        <v>4.0206942623248754E-2</v>
       </c>
     </row>
     <row r="22" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1937,20 +1959,20 @@
       </c>
       <c r="J22" s="39">
         <f t="shared" si="17"/>
-        <v>2.1797413183705729</v>
+        <v>1.1789562579153001</v>
       </c>
       <c r="K22" s="22">
         <f t="shared" si="0"/>
-        <v>3.38404956599926</v>
+        <v>0.7149769203450923</v>
       </c>
       <c r="L22" s="20"/>
       <c r="M22">
         <f t="shared" si="18"/>
-        <v>41.4</v>
+        <v>52.9</v>
       </c>
       <c r="N22" s="2">
         <f t="shared" si="19"/>
-        <v>13803.842646028865</v>
+        <v>194984.45997580478</v>
       </c>
       <c r="O22">
         <v>10</v>
@@ -1967,7 +1989,7 @@
       </c>
       <c r="V22" s="3">
         <f t="shared" si="8"/>
-        <v>7.280261910746999E-2</v>
+        <v>9.4600218053781937E-3</v>
       </c>
     </row>
     <row r="23" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2004,6 +2026,15 @@
       <c r="AG25" s="67"/>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>75</v>
+      </c>
+      <c r="O26">
+        <v>35</v>
+      </c>
+      <c r="P26" t="s">
+        <v>76</v>
+      </c>
       <c r="AB26">
         <v>0</v>
       </c>
@@ -2024,6 +2055,15 @@
       </c>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>70</v>
+      </c>
+      <c r="O27">
+        <v>-31</v>
+      </c>
+      <c r="P27" t="s">
+        <v>6</v>
+      </c>
       <c r="Z27" s="66" t="s">
         <v>23</v>
       </c>
@@ -2050,6 +2090,15 @@
       </c>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>71</v>
+      </c>
+      <c r="O28" s="69">
+        <v>60</v>
+      </c>
+      <c r="P28" t="s">
+        <v>26</v>
+      </c>
       <c r="Z28" s="66"/>
       <c r="AA28" s="6">
         <v>-10</v>
@@ -2074,6 +2123,13 @@
       </c>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <f>O27-O28</f>
+        <v>-91</v>
+      </c>
+      <c r="P29" t="s">
+        <v>6</v>
+      </c>
       <c r="Z29" s="66"/>
       <c r="AA29" s="6">
         <v>-12</v>
@@ -2100,6 +2156,15 @@
     <row r="30" spans="2:33" x14ac:dyDescent="0.25">
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
+      <c r="N30" t="s">
+        <v>2</v>
+      </c>
+      <c r="O30" s="69">
+        <v>51.9</v>
+      </c>
+      <c r="P30" t="s">
+        <v>3</v>
+      </c>
       <c r="Z30" s="66"/>
       <c r="AA30" s="6">
         <v>-14</v>
@@ -2124,6 +2189,13 @@
       </c>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <f>O29-O30</f>
+        <v>-142.9</v>
+      </c>
+      <c r="P31" t="s">
+        <v>6</v>
+      </c>
       <c r="Z31" s="66"/>
       <c r="AA31" s="6">
         <v>-16</v>
@@ -2171,10 +2243,29 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="33" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>72</v>
+      </c>
+      <c r="O33">
+        <v>-174</v>
+      </c>
+      <c r="P33" t="s">
+        <v>73</v>
+      </c>
       <c r="Z33" s="6"/>
     </row>
-    <row r="34" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>74</v>
+      </c>
+      <c r="O34">
+        <f>O31-O33</f>
+        <v>31.099999999999994</v>
+      </c>
+      <c r="P34" t="s">
+        <v>3</v>
+      </c>
       <c r="Z34" s="6"/>
       <c r="AB34" s="68" t="s">
         <v>21</v>
@@ -2185,7 +2276,7 @@
       <c r="AF34" s="68"/>
       <c r="AG34" s="68"/>
     </row>
-    <row r="35" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:33" x14ac:dyDescent="0.25">
       <c r="Z35" s="6"/>
       <c r="AB35" s="67" t="s">
         <v>22</v>
@@ -2196,7 +2287,7 @@
       <c r="AF35" s="67"/>
       <c r="AG35" s="67"/>
     </row>
-    <row r="36" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="14:33" x14ac:dyDescent="0.25">
       <c r="Z36" s="6"/>
       <c r="AB36">
         <v>0</v>
@@ -2217,7 +2308,16 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="37" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>75</v>
+      </c>
+      <c r="O37">
+        <v>915</v>
+      </c>
+      <c r="P37" t="s">
+        <v>76</v>
+      </c>
       <c r="Z37" s="66" t="s">
         <v>23</v>
       </c>
@@ -2243,7 +2343,16 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="38" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>70</v>
+      </c>
+      <c r="O38">
+        <v>-54</v>
+      </c>
+      <c r="P38" t="s">
+        <v>6</v>
+      </c>
       <c r="Z38" s="66"/>
       <c r="AA38" s="6">
         <v>-10</v>
@@ -2267,7 +2376,16 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="39" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>71</v>
+      </c>
+      <c r="O39" s="69">
+        <v>60</v>
+      </c>
+      <c r="P39" t="s">
+        <v>26</v>
+      </c>
       <c r="Z39" s="66"/>
       <c r="AA39" s="6">
         <v>-12</v>
@@ -2291,7 +2409,14 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="40" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <f>O38-O39</f>
+        <v>-114</v>
+      </c>
+      <c r="P40" t="s">
+        <v>6</v>
+      </c>
       <c r="Z40" s="66"/>
       <c r="AA40" s="6">
         <v>-14</v>
@@ -2315,7 +2440,16 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="41" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>2</v>
+      </c>
+      <c r="O41" s="69">
+        <v>28.9</v>
+      </c>
+      <c r="P41" t="s">
+        <v>3</v>
+      </c>
       <c r="Z41" s="66"/>
       <c r="AA41" s="6">
         <v>-16</v>
@@ -2339,7 +2473,14 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="42" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <f>O40-O41</f>
+        <v>-142.9</v>
+      </c>
+      <c r="P42" t="s">
+        <v>6</v>
+      </c>
       <c r="Z42" s="66"/>
       <c r="AA42" s="6">
         <v>-18</v>
@@ -2363,10 +2504,19 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="43" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="14:33" x14ac:dyDescent="0.25">
       <c r="Z43" s="6"/>
     </row>
-    <row r="44" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>72</v>
+      </c>
+      <c r="O44">
+        <v>-174</v>
+      </c>
+      <c r="P44" t="s">
+        <v>73</v>
+      </c>
       <c r="Z44" s="6"/>
       <c r="AB44" s="68" t="s">
         <v>25</v>
@@ -2377,7 +2527,17 @@
       <c r="AF44" s="68"/>
       <c r="AG44" s="68"/>
     </row>
-    <row r="45" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="14:33" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>74</v>
+      </c>
+      <c r="O45">
+        <f>O42-O44</f>
+        <v>31.099999999999994</v>
+      </c>
+      <c r="P45" t="s">
+        <v>3</v>
+      </c>
       <c r="Z45" s="6"/>
       <c r="AB45" s="67" t="s">
         <v>22</v>
@@ -2388,7 +2548,7 @@
       <c r="AF45" s="67"/>
       <c r="AG45" s="67"/>
     </row>
-    <row r="46" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="14:33" x14ac:dyDescent="0.25">
       <c r="Z46" s="6"/>
       <c r="AB46">
         <v>0</v>
@@ -2409,7 +2569,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="47" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="14:33" x14ac:dyDescent="0.25">
       <c r="Z47" s="66" t="s">
         <v>23</v>
       </c>
@@ -2435,7 +2595,7 @@
         <v>-20.8</v>
       </c>
     </row>
-    <row r="48" spans="26:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="14:33" x14ac:dyDescent="0.25">
       <c r="Z48" s="66"/>
       <c r="AA48" s="6">
         <v>-10</v>

</xml_diff>

<commit_message>
zener installed backwards updated transmitter link budget fixed DAC output compliance resistors misc changes on TX chain (see Rev2B)
</commit_message>
<xml_diff>
--- a/docs/graviton_master.xlsx
+++ b/docs/graviton_master.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="81">
   <si>
     <t xml:space="preserve">Graviton Receiver Analog Front End Cascade Analysis </t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>transformer</t>
+  </si>
+  <si>
+    <t>meas</t>
+  </si>
+  <si>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>diff</t>
   </si>
 </sst>
 </file>
@@ -4442,10 +4451,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E9:G32"/>
+  <dimension ref="E9:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4453,15 +4462,30 @@
     <col min="5" max="5" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="K10" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E11" s="5" t="s">
         <v>49</v>
       </c>
@@ -4471,8 +4495,20 @@
       <c r="G11" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="68">
+        <f>F11</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="K11">
+        <f>-32.9+30+3</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E12" s="5" t="s">
         <v>66</v>
       </c>
@@ -4482,8 +4518,20 @@
       <c r="G12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="69">
+        <f>H11+F12</f>
+        <v>-0.5</v>
+      </c>
+      <c r="K12" s="73"/>
+      <c r="L12" t="s">
+        <v>3</v>
+      </c>
+      <c r="M12" s="69">
+        <f>K11+F12</f>
+        <v>-1.3999999999999986</v>
+      </c>
+    </row>
+    <row r="13" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E13" s="5" t="s">
         <v>77</v>
       </c>
@@ -4493,8 +4541,20 @@
       <c r="G13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="69">
+        <f t="shared" ref="H13:H19" si="0">H12+F13</f>
+        <v>-0.85</v>
+      </c>
+      <c r="K13" s="73"/>
+      <c r="L13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" s="69">
+        <f>M12+F13</f>
+        <v>-1.7499999999999987</v>
+      </c>
+    </row>
+    <row r="14" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E14" s="5" t="s">
         <v>71</v>
       </c>
@@ -4504,8 +4564,24 @@
       <c r="G14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="69">
+        <f t="shared" si="0"/>
+        <v>-7.85</v>
+      </c>
+      <c r="K14" s="68">
+        <f>-38.3+30</f>
+        <v>-8.2999999999999972</v>
+      </c>
+      <c r="L14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="69">
+        <f>M13+F14</f>
+        <v>-8.7499999999999982</v>
+      </c>
+      <c r="N14" s="69"/>
+    </row>
+    <row r="15" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E15" s="64" t="s">
         <v>67</v>
       </c>
@@ -4515,99 +4591,189 @@
       <c r="G15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="69">
-        <v>24</v>
+      <c r="H15" s="69">
+        <f t="shared" si="0"/>
+        <v>-8.25</v>
+      </c>
+      <c r="K15" s="68"/>
+      <c r="L15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" s="69">
+        <f>K14+F15</f>
+        <v>-8.6999999999999975</v>
+      </c>
+    </row>
+    <row r="16" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E16" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="68">
+        <v>-2</v>
       </c>
       <c r="G16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="69">
+        <f t="shared" si="0"/>
+        <v>-10.25</v>
+      </c>
+      <c r="K16" s="68"/>
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="69">
+        <f>N15+F16</f>
+        <v>-10.699999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F17" s="69">
-        <v>-2</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="69">
+        <f t="shared" si="0"/>
+        <v>13.75</v>
+      </c>
+      <c r="K17" s="69"/>
+      <c r="L17" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" s="69">
+        <f>N16+F17</f>
+        <v>13.300000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F18" s="69">
-        <v>15.6</v>
+        <v>-2</v>
       </c>
       <c r="G18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="70"/>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="66" t="s">
+      <c r="H18" s="69">
+        <f t="shared" si="0"/>
+        <v>11.75</v>
+      </c>
+      <c r="K18" s="69"/>
+      <c r="L18" t="s">
+        <v>3</v>
+      </c>
+      <c r="N18" s="69">
+        <f>N17+F18</f>
+        <v>11.300000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="69">
+        <v>15.6</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="69">
+        <f t="shared" si="0"/>
+        <v>27.35</v>
+      </c>
+      <c r="K19" s="69"/>
+      <c r="L19" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" s="69">
+        <f>N18+F19</f>
+        <v>26.900000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F20" s="70"/>
+      <c r="K20" s="70"/>
+    </row>
+    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E21" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="71">
-        <f>SUM(F11:F18)</f>
-        <v>29.35</v>
-      </c>
-      <c r="G20" s="66" t="s">
+      <c r="F21" s="71">
+        <f>SUM(F11:F19)</f>
+        <v>27.35</v>
+      </c>
+      <c r="G21" s="66" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F21" s="69"/>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="69">
-        <v>-2</v>
-      </c>
-      <c r="G22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F22" s="69"/>
+      <c r="K22" s="69"/>
+    </row>
+    <row r="23" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>58</v>
       </c>
       <c r="F23" s="69">
-        <v>0.27</v>
+        <v>-0.27</v>
       </c>
       <c r="G23" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="69">
+        <f>H19+F23</f>
+        <v>27.080000000000002</v>
+      </c>
+      <c r="K23" s="69">
+        <v>-0.27</v>
+      </c>
+      <c r="L23" t="s">
+        <v>3</v>
+      </c>
+      <c r="N23" s="69">
+        <f>N19+K23</f>
+        <v>26.630000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F24" s="70"/>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="K24" s="70"/>
+    </row>
+    <row r="25" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E25" s="66" t="s">
         <v>48</v>
       </c>
       <c r="F25" s="71">
-        <f>SUM(F20:F24)</f>
-        <v>27.62</v>
+        <f>SUM(F21:F24)</f>
+        <v>27.080000000000002</v>
       </c>
       <c r="G25" s="66" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F26" s="69"/>
-    </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="K26" s="69"/>
+    </row>
+    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>60</v>
       </c>
@@ -4617,23 +4783,42 @@
       <c r="G27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="69">
+        <f>H23+F27</f>
+        <v>26.580000000000002</v>
+      </c>
+      <c r="K27" s="69">
+        <v>-0.5</v>
+      </c>
+      <c r="L27" t="s">
+        <v>76</v>
+      </c>
+      <c r="N27" s="69">
+        <f>N23+K27</f>
+        <v>26.130000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="5:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="72"/>
-    </row>
-    <row r="29" spans="5:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="72"/>
+    </row>
+    <row r="29" spans="5:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>68</v>
       </c>
       <c r="F29" s="69">
         <f>F25+F27</f>
-        <v>27.12</v>
+        <v>26.580000000000002</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="K29" s="69"/>
+      <c r="L29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>65</v>
       </c>
@@ -4644,16 +4829,30 @@
       <c r="G30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="K30" s="69">
+        <v>25</v>
+      </c>
+      <c r="L30" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="69">
+        <f>K30-N27</f>
+        <v>-1.1300000000000026</v>
+      </c>
+    </row>
+    <row r="32" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>69</v>
       </c>
       <c r="F32" s="65">
         <f>F29-F30</f>
-        <v>2.6500000000000021</v>
+        <v>2.110000000000003</v>
       </c>
       <c r="G32" t="s">
+        <v>3</v>
+      </c>
+      <c r="K32" s="65"/>
+      <c r="L32" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* nightly commit * most everything placed in schematics * major things are to review buck converters
</commit_message>
<xml_diff>
--- a/docs/graviton_master.xlsx
+++ b/docs/graviton_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E25743B3-E4F6-2D4E-8C8F-72C3DF0FFA53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{71AA6B01-53DC-FF42-8B0E-C7C3096A224E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="480" windowWidth="51200" windowHeight="28340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9940" yWindow="5580" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rx_chain" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="134">
   <si>
     <t xml:space="preserve">Graviton Receiver Analog Front End Cascade Analysis </t>
   </si>
@@ -165,12 +165,6 @@
     <t>watts</t>
   </si>
   <si>
-    <t>ADC Digital</t>
-  </si>
-  <si>
-    <t>DAC Digital</t>
-  </si>
-  <si>
     <t>MCU/PHY</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>29V Supply</t>
   </si>
   <si>
-    <t>5V supply</t>
-  </si>
-  <si>
     <t>TX PA #1</t>
   </si>
   <si>
@@ -267,9 +258,6 @@
     <t>antenna IL</t>
   </si>
   <si>
-    <t>cable IL</t>
-  </si>
-  <si>
     <t>connector IL</t>
   </si>
   <si>
@@ -388,6 +376,60 @@
   </si>
   <si>
     <t>IF amp only</t>
+  </si>
+  <si>
+    <t>helical filter</t>
+  </si>
+  <si>
+    <t>SigCarrier</t>
+  </si>
+  <si>
+    <t>3.7V supply</t>
+  </si>
+  <si>
+    <t>-5.5V Supply</t>
+  </si>
+  <si>
+    <t>-5.5V  supply</t>
+  </si>
+  <si>
+    <t>5.5V supply</t>
+  </si>
+  <si>
+    <t>ADC Digital 1.8</t>
+  </si>
+  <si>
+    <t>ADC Analog 1.8</t>
+  </si>
+  <si>
+    <t>ADC Analog 3.3</t>
+  </si>
+  <si>
+    <t>DAC Digital 1.2</t>
+  </si>
+  <si>
+    <t>DAC Digital 3.3</t>
+  </si>
+  <si>
+    <t>DAC Analog 1.2</t>
+  </si>
+  <si>
+    <t>2.5V Rail (ETH, CS VCCIO)</t>
+  </si>
+  <si>
+    <t>1.8V Rail (CS VCCIO)</t>
+  </si>
+  <si>
+    <t>AFE #1 5V</t>
+  </si>
+  <si>
+    <t>AFE #1 -5V</t>
+  </si>
+  <si>
+    <t>AFE #2 5V</t>
+  </si>
+  <si>
+    <t>AFE #2 -5V</t>
   </si>
 </sst>
 </file>
@@ -830,7 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -936,6 +978,22 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -945,22 +1003,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1690,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="160" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1761,7 +1808,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H2" s="80">
         <v>35000000</v>
@@ -1794,7 +1841,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H3" s="80">
         <f>125000000/4096</f>
@@ -1828,7 +1875,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H4" s="79">
         <f>-174+10*LOG10(H3)</f>
@@ -1916,7 +1963,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>25</v>
@@ -2038,11 +2085,11 @@
     </row>
     <row r="9" spans="1:27" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="13">
@@ -2080,11 +2127,11 @@
       <c r="P9" s="17"/>
       <c r="Q9" s="18">
         <f>Q10-E9</f>
-        <v>-43.67</v>
+        <v>-42.67</v>
       </c>
       <c r="R9" s="19">
         <f t="shared" ref="R9:R28" si="1">10^((Q9-30)/10)*1000000</f>
-        <v>4.2953642676488643E-2</v>
+        <v>5.4075432294557912E-2</v>
       </c>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -2098,11 +2145,11 @@
     </row>
     <row r="10" spans="1:27" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="20">
@@ -2142,11 +2189,11 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="24">
         <f t="shared" ref="Q10:Q27" si="3">Q11-E10</f>
-        <v>-43.67</v>
+        <v>-42.67</v>
       </c>
       <c r="R10" s="30">
         <f t="shared" si="1"/>
-        <v>4.2953642676488643E-2</v>
+        <v>5.4075432294557912E-2</v>
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -2163,62 +2210,62 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="35" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="20">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F11" s="21">
         <f t="shared" ref="F11:F12" si="4">10^(E11/10)</f>
-        <v>1</v>
+        <v>0.79432823472428149</v>
       </c>
       <c r="G11" s="22">
         <f t="shared" ref="G11:G12" si="5">ABS(E11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="23">
         <f t="shared" ref="H11:H12" si="6">10^(G11/10)</f>
-        <v>1</v>
+        <v>1.2589254117941673</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="24">
         <f t="shared" ref="J11:J12" si="7">J10+((H11-1)/N10)</f>
-        <v>1</v>
+        <v>1.2589254117941673</v>
       </c>
       <c r="K11" s="24">
         <f t="shared" ref="K11:K12" si="8">10*LOG10(J11)</f>
-        <v>0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="L11" s="24"/>
       <c r="M11" s="3">
         <f t="shared" ref="M11:M12" si="9">E11+M10</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N11" s="24">
         <f t="shared" ref="N11:N12" si="10">N10*F11</f>
-        <v>1</v>
+        <v>0.79432823472428149</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="24">
         <f t="shared" si="3"/>
-        <v>-43.67</v>
+        <v>-42.67</v>
       </c>
       <c r="R11" s="30">
         <f t="shared" si="1"/>
-        <v>4.2953642676488643E-2</v>
+        <v>5.4075432294557912E-2</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="25">
         <f t="shared" ref="V11:V14" si="11">K11-K10</f>
-        <v>0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
@@ -2228,13 +2275,13 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B12" s="70">
         <v>132136</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="20">
@@ -2255,20 +2302,20 @@
       <c r="I12" s="3"/>
       <c r="J12" s="24">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>1.2589254117941673</v>
       </c>
       <c r="K12" s="24">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="L12" s="24"/>
       <c r="M12" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N12" s="24">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.79432823472428149</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -2295,13 +2342,13 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="20">
@@ -2322,20 +2369,20 @@
       <c r="I13" s="3"/>
       <c r="J13" s="24">
         <f t="shared" ref="J13:J27" si="13">J12+((H13-1)/N12)</f>
-        <v>1.0715193052376064</v>
+        <v>1.3489628825916538</v>
       </c>
       <c r="K13" s="24">
         <f t="shared" ref="K13:K27" si="14">10*LOG10(J13)</f>
-        <v>0.3</v>
+        <v>1.3000000000000007</v>
       </c>
       <c r="L13" s="24"/>
       <c r="M13" s="3">
         <f t="shared" ref="M13:M27" si="15">E13+M12</f>
-        <v>-0.3</v>
+        <v>-1.3</v>
       </c>
       <c r="N13" s="24">
         <f t="shared" ref="N13:N27" si="16">N12*F13</f>
-        <v>0.93325430079699101</v>
+        <v>0.74131024130091749</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -2352,7 +2399,7 @@
       <c r="U13" s="3"/>
       <c r="V13" s="25">
         <f t="shared" si="11"/>
-        <v>0.3</v>
+        <v>0.30000000000000049</v>
       </c>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -2362,10 +2409,10 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C14" s="67" t="s">
         <v>17</v>
@@ -2388,20 +2435,20 @@
       <c r="I14" s="3"/>
       <c r="J14" s="24">
         <f t="shared" si="13"/>
-        <v>1.1297959146727978</v>
+        <v>1.4223287871228198</v>
       </c>
       <c r="K14" s="24">
         <f t="shared" si="14"/>
-        <v>0.53</v>
+        <v>1.5300000000000002</v>
       </c>
       <c r="L14" s="24"/>
       <c r="M14" s="3">
         <f t="shared" si="15"/>
-        <v>20.2</v>
+        <v>19.2</v>
       </c>
       <c r="N14" s="24">
         <f t="shared" si="16"/>
-        <v>104.71285480508995</v>
+        <v>83.176377110267097</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -2418,7 +2465,7 @@
       <c r="U14" s="3"/>
       <c r="V14" s="25">
         <f t="shared" si="11"/>
-        <v>0.23000000000000004</v>
+        <v>0.22999999999999954</v>
       </c>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -2428,13 +2475,13 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="67" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="20">
@@ -2455,20 +2502,20 @@
       <c r="I15" s="3"/>
       <c r="J15" s="24">
         <f t="shared" si="13"/>
-        <v>1.1353816012969455</v>
+        <v>1.4293607499562782</v>
       </c>
       <c r="K15" s="24">
         <f t="shared" si="14"/>
-        <v>0.55141852263929469</v>
+        <v>1.5514185226392949</v>
       </c>
       <c r="L15" s="24"/>
       <c r="M15" s="3">
         <f t="shared" si="15"/>
-        <v>18.2</v>
+        <v>17.2</v>
       </c>
       <c r="N15" s="24">
         <f t="shared" si="16"/>
-        <v>66.069344800759595</v>
+        <v>52.480746024977257</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -2495,7 +2542,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>27</v>
@@ -2522,20 +2569,20 @@
       <c r="I16" s="3"/>
       <c r="J16" s="24">
         <f t="shared" si="13"/>
-        <v>1.1372284253372009</v>
+        <v>1.431685763671668</v>
       </c>
       <c r="K16" s="24">
         <f t="shared" si="14"/>
-        <v>0.55847706464067903</v>
+        <v>1.5584770646406789</v>
       </c>
       <c r="L16" s="24"/>
       <c r="M16" s="3">
         <f t="shared" si="15"/>
-        <v>17.7</v>
+        <v>16.7</v>
       </c>
       <c r="N16" s="24">
         <f t="shared" si="16"/>
-        <v>58.884365535558885</v>
+        <v>46.77351412871981</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -2552,7 +2599,7 @@
       <c r="U16" s="3"/>
       <c r="V16" s="25">
         <f t="shared" si="19"/>
-        <v>7.0585420013843381E-3</v>
+        <v>7.058542001384005E-3</v>
       </c>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -2562,13 +2609,13 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="67" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="20">
@@ -2589,20 +2636,20 @@
       <c r="I17" s="3"/>
       <c r="J17" s="24">
         <f t="shared" si="13"/>
-        <v>1.1471613368518527</v>
+        <v>1.4441905583905659</v>
       </c>
       <c r="K17" s="24">
         <f t="shared" si="14"/>
-        <v>0.59624501403528196</v>
+        <v>1.5962450140352813</v>
       </c>
       <c r="L17" s="24"/>
       <c r="M17" s="3">
         <f t="shared" si="15"/>
-        <v>15.7</v>
+        <v>14.7</v>
       </c>
       <c r="N17" s="24">
         <f t="shared" si="16"/>
-        <v>37.153522909717246</v>
+        <v>29.512092266663853</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -2619,7 +2666,7 @@
       <c r="U17" s="3"/>
       <c r="V17" s="25">
         <f t="shared" si="19"/>
-        <v>3.7767949394602929E-2</v>
+        <v>3.7767949394602374E-2</v>
       </c>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -2629,10 +2676,10 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C18" s="67" t="s">
         <v>17</v>
@@ -2655,20 +2702,20 @@
       <c r="I18" s="3"/>
       <c r="J18" s="24">
         <f t="shared" si="13"/>
-        <v>1.1486251790969992</v>
+        <v>1.4460334265918384</v>
       </c>
       <c r="K18" s="24">
         <f t="shared" si="14"/>
-        <v>0.60178332250763344</v>
+        <v>1.6017833225076323</v>
       </c>
       <c r="L18" s="24"/>
       <c r="M18" s="3">
         <f t="shared" si="15"/>
-        <v>36.200000000000003</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="N18" s="24">
         <f t="shared" si="16"/>
-        <v>4168.6938347033529</v>
+        <v>3311.3112148259106</v>
       </c>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
@@ -2685,7 +2732,7 @@
       <c r="U18" s="3"/>
       <c r="V18" s="25">
         <f t="shared" si="19"/>
-        <v>5.538308472351483E-3</v>
+        <v>5.538308472351039E-3</v>
       </c>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
@@ -2695,7 +2742,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" s="78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B19" s="71" t="s">
         <v>30</v>
@@ -2721,20 +2768,20 @@
       <c r="I19" s="68"/>
       <c r="J19" s="72">
         <f t="shared" si="13"/>
-        <v>1.1495875602397148</v>
+        <v>1.4472449926682345</v>
       </c>
       <c r="K19" s="72">
         <f t="shared" si="14"/>
-        <v>0.60542055623317403</v>
+        <v>1.6054205562331727</v>
       </c>
       <c r="L19" s="72"/>
       <c r="M19" s="68">
         <f t="shared" si="15"/>
-        <v>29.200000000000003</v>
+        <v>28.200000000000003</v>
       </c>
       <c r="N19" s="72">
         <f t="shared" si="16"/>
-        <v>831.76377110267072</v>
+        <v>660.69344800759586</v>
       </c>
       <c r="O19" s="68">
         <v>0</v>
@@ -2760,7 +2807,7 @@
       </c>
       <c r="V19" s="75">
         <f t="shared" si="19"/>
-        <v>3.6372337255405895E-3</v>
+        <v>3.6372337255403675E-3</v>
       </c>
       <c r="W19" s="27" t="s">
         <v>9</v>
@@ -2772,7 +2819,7 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" s="78" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>24</v>
@@ -2799,20 +2846,20 @@
       <c r="I20" s="3"/>
       <c r="J20" s="24">
         <f t="shared" si="13"/>
-        <v>1.1500448827125349</v>
+        <v>1.4478207275506523</v>
       </c>
       <c r="K20" s="24">
         <f t="shared" si="14"/>
-        <v>0.60714789861454543</v>
+        <v>1.607147898614544</v>
       </c>
       <c r="L20" s="24"/>
       <c r="M20" s="3">
         <f t="shared" si="15"/>
-        <v>27.800000000000004</v>
+        <v>26.800000000000004</v>
       </c>
       <c r="N20" s="24">
         <f t="shared" si="16"/>
-        <v>602.55958607435753</v>
+        <v>478.63009232263829</v>
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
@@ -2829,7 +2876,7 @@
       <c r="U20" s="3"/>
       <c r="V20" s="25">
         <f t="shared" si="19"/>
-        <v>1.7273423813713995E-3</v>
+        <v>1.7273423813712885E-3</v>
       </c>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
@@ -2839,13 +2886,13 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="1">
@@ -2866,20 +2913,20 @@
       <c r="I21" s="3"/>
       <c r="J21" s="24">
         <f t="shared" si="13"/>
-        <v>1.1516966070199233</v>
+        <v>1.4499001252545016</v>
       </c>
       <c r="K21" s="24">
         <f t="shared" si="14"/>
-        <v>0.61338087376535011</v>
+        <v>1.6133808737653488</v>
       </c>
       <c r="L21" s="24"/>
       <c r="M21" s="24">
         <f t="shared" si="15"/>
-        <v>24.800000000000004</v>
+        <v>23.800000000000004</v>
       </c>
       <c r="N21" s="24">
         <f t="shared" si="16"/>
-        <v>301.99517204020151</v>
+        <v>239.88329190194901</v>
       </c>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
@@ -2896,7 +2943,7 @@
       <c r="U21" s="3"/>
       <c r="V21" s="25">
         <f t="shared" ref="V21" si="25">K21-K20</f>
-        <v>6.232975150804676E-3</v>
+        <v>6.232975150804787E-3</v>
       </c>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
@@ -2906,7 +2953,7 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>22</v>
@@ -2922,7 +2969,7 @@
         <f t="shared" si="12"/>
         <v>22.233098906514034</v>
       </c>
-      <c r="G22" s="89">
+      <c r="G22" s="86">
         <v>10</v>
       </c>
       <c r="H22" s="23">
@@ -2932,20 +2979,20 @@
       <c r="I22" s="3"/>
       <c r="J22" s="24">
         <f t="shared" si="13"/>
-        <v>1.1814984079533564</v>
+        <v>1.4874183697668317</v>
       </c>
       <c r="K22" s="24">
         <f t="shared" si="14"/>
-        <v>0.72433140765223958</v>
+        <v>1.7243314076522385</v>
       </c>
       <c r="L22" s="24"/>
       <c r="M22" s="24">
         <f t="shared" si="15"/>
-        <v>38.270000000000003</v>
+        <v>37.270000000000003</v>
       </c>
       <c r="N22" s="24">
         <f t="shared" si="16"/>
-        <v>6714.288529259522</v>
+        <v>5333.3489548762091</v>
       </c>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
@@ -2962,7 +3009,7 @@
       <c r="U22" s="3"/>
       <c r="V22" s="25">
         <f>K22-K20</f>
-        <v>0.11718350903769414</v>
+        <v>0.11718350903769448</v>
       </c>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
@@ -2972,13 +3019,13 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C23" s="69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="29">
@@ -2999,20 +3046,20 @@
       <c r="I23" s="3"/>
       <c r="J23" s="24">
         <f t="shared" si="13"/>
-        <v>1.181510907701268</v>
+        <v>1.4874341060171186</v>
       </c>
       <c r="K23" s="24">
         <f t="shared" si="14"/>
-        <v>0.72437735390820457</v>
+        <v>1.724377353908203</v>
       </c>
       <c r="L23" s="24"/>
       <c r="M23" s="24">
         <f t="shared" si="15"/>
-        <v>37.92</v>
+        <v>36.92</v>
       </c>
       <c r="N23" s="24">
         <f t="shared" si="16"/>
-        <v>6194.4107507678127</v>
+        <v>4920.3953568145089</v>
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -3029,7 +3076,7 @@
       <c r="U23" s="3"/>
       <c r="V23" s="25">
         <f t="shared" ref="V23:V29" si="26">K23-K21</f>
-        <v>0.11099648014285446</v>
+        <v>0.11099648014285424</v>
       </c>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
@@ -3039,13 +3086,13 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C24" s="67" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="1">
@@ -3066,20 +3113,20 @@
       <c r="I24" s="3"/>
       <c r="J24" s="24">
         <f t="shared" si="13"/>
-        <v>1.181510907701268</v>
+        <v>1.4874341060171186</v>
       </c>
       <c r="K24" s="24">
         <f t="shared" si="14"/>
-        <v>0.72437735390820457</v>
+        <v>1.724377353908203</v>
       </c>
       <c r="L24" s="24"/>
       <c r="M24" s="24">
         <f t="shared" si="15"/>
-        <v>37.92</v>
+        <v>36.92</v>
       </c>
       <c r="N24" s="24">
         <f t="shared" si="16"/>
-        <v>6194.4107507678127</v>
+        <v>4920.3953568145089</v>
       </c>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
@@ -3096,7 +3143,7 @@
       <c r="U24" s="3"/>
       <c r="V24" s="25">
         <f t="shared" si="26"/>
-        <v>4.5946255964990357E-5</v>
+        <v>4.5946255964546268E-5</v>
       </c>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
@@ -3106,7 +3153,7 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B25" s="66" t="s">
         <v>22</v>
@@ -3122,7 +3169,7 @@
         <f t="shared" si="12"/>
         <v>22.233098906514034</v>
       </c>
-      <c r="G25" s="89">
+      <c r="G25" s="86">
         <v>10</v>
       </c>
       <c r="H25" s="23">
@@ -3132,20 +3179,20 @@
       <c r="I25" s="3"/>
       <c r="J25" s="24">
         <f t="shared" si="13"/>
-        <v>1.1829638304024119</v>
+        <v>1.4892632273269613</v>
       </c>
       <c r="K25" s="24">
         <f t="shared" si="14"/>
-        <v>0.72971466101484173</v>
+        <v>1.7297146610148402</v>
       </c>
       <c r="L25" s="24"/>
       <c r="M25" s="24">
         <f t="shared" si="15"/>
-        <v>51.39</v>
+        <v>50.39</v>
       </c>
       <c r="N25" s="24">
         <f t="shared" si="16"/>
-        <v>137720.94688939463</v>
+        <v>109395.63662720939</v>
       </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
@@ -3172,13 +3219,13 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B26" s="66" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C26" s="69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="1">
@@ -3199,20 +3246,20 @@
       <c r="I26" s="3"/>
       <c r="J26" s="24">
         <f t="shared" si="13"/>
-        <v>1.1829632681889317</v>
+        <v>1.4892625195421243</v>
       </c>
       <c r="K26" s="24">
         <f t="shared" si="14"/>
-        <v>0.72971259699340796</v>
+        <v>1.7297125969934066</v>
       </c>
       <c r="L26" s="24"/>
       <c r="M26" s="24">
         <f t="shared" si="15"/>
-        <v>51.04</v>
+        <v>50.04</v>
       </c>
       <c r="N26" s="24">
         <f t="shared" si="16"/>
-        <v>127057.41052085414</v>
+        <v>100925.28860766844</v>
       </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -3229,7 +3276,7 @@
       <c r="U26" s="3"/>
       <c r="V26" s="25">
         <f t="shared" si="26"/>
-        <v>5.3352430852033894E-3</v>
+        <v>5.3352430852036115E-3</v>
       </c>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
@@ -3239,13 +3286,13 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B27" s="66" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" s="67" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="1">
@@ -3266,20 +3313,20 @@
       <c r="I27" s="3"/>
       <c r="J27" s="24">
         <f t="shared" si="13"/>
-        <v>1.1829632681889317</v>
+        <v>1.4892625195421243</v>
       </c>
       <c r="K27" s="24">
         <f t="shared" si="14"/>
-        <v>0.72971259699340796</v>
+        <v>1.7297125969934066</v>
       </c>
       <c r="L27" s="24"/>
       <c r="M27" s="24">
         <f t="shared" si="15"/>
-        <v>51.04</v>
+        <v>50.04</v>
       </c>
       <c r="N27" s="24">
         <f t="shared" si="16"/>
-        <v>127057.41052085414</v>
+        <v>100925.28860766844</v>
       </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -3296,7 +3343,7 @@
       <c r="U27" s="3"/>
       <c r="V27" s="25">
         <f t="shared" si="26"/>
-        <v>-2.0640214337674934E-6</v>
+        <v>-2.0640214335454488E-6</v>
       </c>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
@@ -3306,13 +3353,13 @@
     </row>
     <row r="28" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="35" t="s">
         <v>65</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>68</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="1">
@@ -3333,20 +3380,20 @@
       <c r="I28" s="3"/>
       <c r="J28" s="24">
         <f t="shared" ref="J28:J29" si="28">J27+((H28-1)/N27)</f>
-        <v>1.182963968109487</v>
+        <v>1.4892634006898977</v>
       </c>
       <c r="K28" s="24">
         <f t="shared" ref="K28:K29" si="29">10*LOG10(J28)</f>
-        <v>0.7297151665706143</v>
+        <v>1.7297151665706134</v>
       </c>
       <c r="L28" s="24"/>
       <c r="M28" s="24">
         <f t="shared" ref="M28:M29" si="30">E28+M27</f>
-        <v>50.67</v>
+        <v>49.67</v>
       </c>
       <c r="N28" s="24">
         <f t="shared" ref="N28:N29" si="31">N27*F28</f>
-        <v>116680.96170609623</v>
+        <v>92682.982337934925</v>
       </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -3363,7 +3410,7 @@
       <c r="U28" s="3"/>
       <c r="V28" s="25">
         <f t="shared" si="26"/>
-        <v>2.5695772063460964E-6</v>
+        <v>2.5695772067901856E-6</v>
       </c>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
@@ -3377,7 +3424,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="20">
@@ -3397,20 +3444,20 @@
       <c r="I29" s="3"/>
       <c r="J29" s="25">
         <f t="shared" si="28"/>
-        <v>1.1872507619986836</v>
-      </c>
-      <c r="K29" s="88">
+        <v>1.4946601544521312</v>
+      </c>
+      <c r="K29" s="85">
         <f t="shared" si="29"/>
-        <v>0.74542456992078554</v>
+        <v>1.7454245699207842</v>
       </c>
       <c r="L29" s="24"/>
       <c r="M29" s="24">
         <f t="shared" si="30"/>
-        <v>50.67</v>
+        <v>49.67</v>
       </c>
       <c r="N29" s="24">
         <f t="shared" si="31"/>
-        <v>116680.96170609623</v>
+        <v>92682.982337934925</v>
       </c>
       <c r="O29" s="3">
         <v>9</v>
@@ -4279,8 +4326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C7:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="177" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A8" zoomScale="177" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4300,8 +4347,8 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.2">
       <c r="F9" s="39"/>
@@ -4309,49 +4356,49 @@
       <c r="H9" s="39"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C10" s="95" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="95" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="95" t="s">
+      <c r="C10" s="91" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="94" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="94" t="s">
-        <v>113</v>
-      </c>
-      <c r="H10" s="94" t="s">
-        <v>114</v>
+      <c r="F10" s="90" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="90" t="s">
+        <v>110</v>
       </c>
       <c r="I10" s="40"/>
-      <c r="J10" s="95" t="s">
+      <c r="J10" s="91" t="s">
+        <v>107</v>
+      </c>
+      <c r="K10" s="40"/>
+      <c r="L10" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="95" t="s">
-        <v>115</v>
-      </c>
-      <c r="M10" s="95" t="s">
-        <v>100</v>
-      </c>
-      <c r="N10" s="95" t="s">
-        <v>99</v>
-      </c>
-      <c r="O10" s="95" t="s">
-        <v>98</v>
-      </c>
-      <c r="P10" s="85"/>
+      <c r="M10" s="91" t="s">
+        <v>96</v>
+      </c>
+      <c r="N10" s="91" t="s">
+        <v>95</v>
+      </c>
+      <c r="O10" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="P10" s="82"/>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="D11" s="92" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="84" t="s">
-        <v>87</v>
+      <c r="D11" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="81" t="s">
+        <v>83</v>
       </c>
       <c r="F11" s="42">
         <v>6.99</v>
@@ -4371,7 +4418,7 @@
       </c>
       <c r="K11" s="44"/>
       <c r="L11" s="38">
-        <f>10^(J11/10)/1000</f>
+        <f t="shared" ref="L11:L19" si="0">10^(J11/10)/1000</f>
         <v>5.0003453497697867E-3</v>
       </c>
       <c r="M11" s="38">
@@ -4387,13 +4434,13 @@
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C12" s="85" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="93" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="84" t="s">
+      <c r="C12" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="81" t="s">
         <v>38</v>
       </c>
       <c r="F12" s="42">
@@ -4405,37 +4452,37 @@
       <c r="H12" s="42">
         <v>-0.4</v>
       </c>
-      <c r="I12" s="84" t="s">
+      <c r="I12" s="81" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="44">
-        <f>J11+F12</f>
+        <f t="shared" ref="J12:J19" si="1">J11+F12</f>
         <v>6.6400000000000006</v>
       </c>
       <c r="K12" s="44"/>
       <c r="L12" s="38">
-        <f>10^(J12/10)/1000</f>
+        <f t="shared" si="0"/>
         <v>4.6131757456037946E-3</v>
       </c>
       <c r="M12" s="38">
         <v>200</v>
       </c>
       <c r="N12" s="38">
-        <f t="shared" ref="N12:N17" si="0">SQRT(L12/M12)</f>
+        <f t="shared" ref="N12:N17" si="2">SQRT(L12/M12)</f>
         <v>4.8026949443014779E-3</v>
       </c>
       <c r="O12" s="38">
-        <f t="shared" ref="O12:O17" si="1">SQRT(L12*M12)</f>
+        <f t="shared" ref="O12:O17" si="3">SQRT(L12*M12)</f>
         <v>0.96053898886029554</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C13" s="85"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="86" t="s">
-        <v>105</v>
+        <v>66</v>
+      </c>
+      <c r="E13" s="83" t="s">
+        <v>101</v>
       </c>
       <c r="F13" s="42">
         <v>-1.4</v>
@@ -4446,34 +4493,34 @@
       <c r="H13" s="42">
         <v>0</v>
       </c>
-      <c r="I13" s="84"/>
+      <c r="I13" s="81"/>
       <c r="J13" s="44">
-        <f>J12+F13</f>
+        <f t="shared" si="1"/>
         <v>5.24</v>
       </c>
       <c r="K13" s="44"/>
       <c r="L13" s="38">
-        <f>10^(J13/10)/1000</f>
+        <f t="shared" si="0"/>
         <v>3.3419504002611426E-3</v>
       </c>
       <c r="M13" s="38">
         <v>201</v>
       </c>
       <c r="N13" s="38">
-        <f t="shared" ref="N13" si="2">SQRT(L13/M13)</f>
+        <f t="shared" ref="N13" si="4">SQRT(L13/M13)</f>
         <v>4.0775751258280762E-3</v>
       </c>
       <c r="O13" s="38">
-        <f t="shared" ref="O13" si="3">SQRT(L13*M13)</f>
+        <f t="shared" ref="O13" si="5">SQRT(L13*M13)</f>
         <v>0.81959260029144332</v>
       </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="D14" s="92" t="s">
+      <c r="D14" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="85" t="s">
-        <v>119</v>
+      <c r="E14" s="82" t="s">
+        <v>115</v>
       </c>
       <c r="F14" s="43">
         <v>-14.22</v>
@@ -4488,23 +4535,23 @@
         <v>3</v>
       </c>
       <c r="J14" s="44">
-        <f>J13+F14</f>
+        <f t="shared" si="1"/>
         <v>-8.98</v>
       </c>
       <c r="K14" s="44"/>
       <c r="L14" s="38">
-        <f>10^(J14/10)/1000</f>
+        <f t="shared" si="0"/>
         <v>1.2647363474711513E-4</v>
       </c>
       <c r="M14" s="38">
         <v>50</v>
       </c>
       <c r="N14" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5904316064962688E-3</v>
       </c>
       <c r="O14" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.9521580324813448E-2</v>
       </c>
     </row>
@@ -4515,48 +4562,48 @@
       <c r="E15" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="91">
+      <c r="F15" s="87">
         <v>-1.8</v>
       </c>
-      <c r="G15" s="91">
+      <c r="G15" s="87">
         <v>-1.4</v>
       </c>
-      <c r="H15" s="91">
+      <c r="H15" s="87">
         <v>-1.4</v>
       </c>
       <c r="I15" s="38" t="s">
         <v>3</v>
       </c>
       <c r="J15" s="44">
-        <f>J14+F15</f>
+        <f t="shared" si="1"/>
         <v>-10.780000000000001</v>
       </c>
       <c r="K15" s="44"/>
       <c r="L15" s="38">
-        <f>10^(J15/10)/1000</f>
+        <f t="shared" si="0"/>
         <v>8.3560301823124781E-5</v>
       </c>
       <c r="M15" s="38">
         <v>50</v>
       </c>
       <c r="N15" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2927513436320596E-3</v>
       </c>
       <c r="O15" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.463756718160299E-2</v>
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C16" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="85" t="s">
+      <c r="C16" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="84" t="s">
-        <v>88</v>
+      <c r="E16" s="81" t="s">
+        <v>84</v>
       </c>
       <c r="F16" s="42">
         <v>-7</v>
@@ -4571,35 +4618,35 @@
         <v>3</v>
       </c>
       <c r="J16" s="44">
-        <f>J15+F16</f>
+        <f t="shared" si="1"/>
         <v>-17.78</v>
       </c>
       <c r="K16" s="44"/>
       <c r="L16" s="38">
-        <f>10^(J16/10)/1000</f>
+        <f t="shared" si="0"/>
         <v>1.6672472125510625E-5</v>
       </c>
       <c r="M16" s="38">
         <v>50</v>
       </c>
       <c r="N16" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.7745081393155255E-4</v>
       </c>
       <c r="O16" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.8872540696577628E-2</v>
       </c>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C17" s="85" t="s">
-        <v>108</v>
+      <c r="C17" s="82" t="s">
+        <v>104</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="84" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="E17" s="81" t="s">
+        <v>86</v>
       </c>
       <c r="F17" s="43">
         <v>17.5</v>
@@ -4614,35 +4661,35 @@
         <v>3</v>
       </c>
       <c r="J17" s="44">
-        <f>J16+F17</f>
+        <f t="shared" si="1"/>
         <v>-0.28000000000000114</v>
       </c>
       <c r="K17" s="44"/>
       <c r="L17" s="38">
-        <f>10^(J17/10)/1000</f>
+        <f t="shared" si="0"/>
         <v>9.3756200692587997E-4</v>
       </c>
       <c r="M17" s="38">
         <v>50</v>
       </c>
       <c r="N17" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.3302702154158464E-3</v>
       </c>
       <c r="O17" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.21651351077079231</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C18" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="85" t="s">
+      <c r="C18" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="86" t="s">
-        <v>91</v>
+      <c r="E18" s="83" t="s">
+        <v>87</v>
       </c>
       <c r="F18" s="43">
         <v>-3</v>
@@ -4657,35 +4704,35 @@
         <v>3</v>
       </c>
       <c r="J18" s="44">
-        <f>J17+F18</f>
+        <f t="shared" si="1"/>
         <v>-3.2800000000000011</v>
       </c>
       <c r="K18" s="44"/>
       <c r="L18" s="38">
-        <f>10^(J18/10)/1000</f>
+        <f t="shared" si="0"/>
         <v>4.6989410860521526E-4</v>
       </c>
       <c r="M18" s="38">
         <v>50</v>
       </c>
       <c r="N18" s="38">
-        <f t="shared" ref="N18:N19" si="4">SQRT(L18/M18)</f>
+        <f t="shared" ref="N18:N19" si="6">SQRT(L18/M18)</f>
         <v>3.0655965442478411E-3</v>
       </c>
       <c r="O18" s="38">
-        <f t="shared" ref="O18:O19" si="5">SQRT(L18*M18)</f>
+        <f t="shared" ref="O18:O19" si="7">SQRT(L18*M18)</f>
         <v>0.15327982721239206</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C19" s="85" t="s">
-        <v>108</v>
+      <c r="C19" s="82" t="s">
+        <v>104</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" s="84" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="E19" s="81" t="s">
+        <v>86</v>
       </c>
       <c r="F19" s="43">
         <v>17.5</v>
@@ -4696,39 +4743,39 @@
       <c r="H19" s="43">
         <v>19.5</v>
       </c>
-      <c r="I19" s="85" t="s">
+      <c r="I19" s="82" t="s">
         <v>3</v>
       </c>
       <c r="J19" s="44">
-        <f>J18+F19</f>
+        <f t="shared" si="1"/>
         <v>14.219999999999999</v>
       </c>
       <c r="K19" s="44"/>
       <c r="L19" s="38">
-        <f>10^(J19/10)/1000</f>
+        <f t="shared" si="0"/>
         <v>2.6424087573219474E-2</v>
       </c>
       <c r="M19" s="38">
         <v>50</v>
       </c>
       <c r="N19" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.2988730966810443E-2</v>
       </c>
       <c r="O19" s="38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.1494365483405222</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C20" s="85" t="s">
-        <v>108</v>
+      <c r="C20" s="82" t="s">
+        <v>104</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="86" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="E20" s="83" t="s">
+        <v>86</v>
       </c>
       <c r="F20" s="43">
         <v>16.5</v>
@@ -4739,36 +4786,36 @@
       <c r="H20" s="43">
         <v>17.5</v>
       </c>
-      <c r="I20" s="85" t="s">
+      <c r="I20" s="82" t="s">
         <v>3</v>
       </c>
       <c r="J20" s="44">
-        <f t="shared" ref="J20:J22" si="6">J19+F20</f>
+        <f t="shared" ref="J20:J22" si="8">J19+F20</f>
         <v>30.72</v>
       </c>
       <c r="K20" s="44"/>
       <c r="L20" s="38">
-        <f t="shared" ref="L20:L25" si="7">10^(J20/10)/1000</f>
+        <f t="shared" ref="L20:L25" si="9">10^(J20/10)/1000</f>
         <v>1.1803206356517304</v>
       </c>
       <c r="M20" s="38">
         <v>50</v>
       </c>
       <c r="N20" s="38">
-        <f t="shared" ref="N20:N25" si="8">SQRT(L20/M20)</f>
+        <f t="shared" ref="N20:N25" si="10">SQRT(L20/M20)</f>
         <v>0.1536437851428902</v>
       </c>
       <c r="O20" s="38">
-        <f t="shared" ref="O20:O25" si="9">SQRT(L20*M20)</f>
+        <f t="shared" ref="O20:O25" si="11">SQRT(L20*M20)</f>
         <v>7.6821892571445103</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C21" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="86" t="s">
-        <v>106</v>
+      <c r="C21" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="83" t="s">
+        <v>102</v>
       </c>
       <c r="F21" s="43">
         <v>-3.4</v>
@@ -4779,37 +4826,37 @@
       <c r="H21" s="43">
         <v>-3</v>
       </c>
-      <c r="I21" s="85"/>
+      <c r="I21" s="82"/>
       <c r="J21" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>27.32</v>
       </c>
       <c r="K21" s="44"/>
       <c r="L21" s="38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.53951062251512827</v>
       </c>
       <c r="M21" s="38">
         <v>50</v>
       </c>
       <c r="N21" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.1038759474098916</v>
       </c>
       <c r="O21" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>5.1937973704945799</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C22" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="D22" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="86" t="s">
-        <v>116</v>
+      <c r="C22" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="83" t="s">
+        <v>112</v>
       </c>
       <c r="F22" s="44">
         <v>12.5</v>
@@ -4820,36 +4867,36 @@
       <c r="H22" s="44">
         <v>14</v>
       </c>
-      <c r="I22" s="85" t="s">
+      <c r="I22" s="82" t="s">
         <v>3</v>
       </c>
       <c r="J22" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>39.82</v>
       </c>
       <c r="K22" s="44"/>
       <c r="L22" s="38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9.5940063151593389</v>
       </c>
       <c r="M22" s="38">
         <v>50</v>
       </c>
       <c r="N22" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.43804123813082574</v>
       </c>
       <c r="O22" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>21.902061906541288</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C23" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="86" t="s">
-        <v>110</v>
+      <c r="C23" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="83" t="s">
+        <v>106</v>
       </c>
       <c r="F23" s="44">
         <v>-0.3</v>
@@ -4860,7 +4907,7 @@
       <c r="H23" s="44">
         <v>-0.3</v>
       </c>
-      <c r="I23" s="85" t="s">
+      <c r="I23" s="82" t="s">
         <v>3</v>
       </c>
       <c r="J23" s="44">
@@ -4869,29 +4916,29 @@
       </c>
       <c r="K23" s="44"/>
       <c r="L23" s="38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.101539309541415</v>
       </c>
       <c r="M23" s="38">
         <v>50</v>
       </c>
       <c r="N23" s="38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.14842771368861107</v>
       </c>
       <c r="O23" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>7.421385684430553</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C24" s="85" t="s">
-        <v>108</v>
+      <c r="C24" s="82" t="s">
+        <v>104</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="86" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="83" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="44">
@@ -4903,7 +4950,7 @@
       <c r="H24" s="44">
         <v>-0.3</v>
       </c>
-      <c r="I24" s="85" t="s">
+      <c r="I24" s="82" t="s">
         <v>3</v>
       </c>
       <c r="J24" s="44">
@@ -4912,59 +4959,59 @@
       </c>
       <c r="K24" s="44"/>
       <c r="L24" s="38">
-        <f t="shared" ref="L24" si="10">10^(J24/10)/1000</f>
+        <f t="shared" ref="L24" si="12">10^(J24/10)/1000</f>
         <v>0.50350060878790504</v>
       </c>
       <c r="M24" s="38">
         <v>50</v>
       </c>
       <c r="N24" s="38">
-        <f t="shared" ref="N24" si="11">SQRT(L24/M24)</f>
+        <f t="shared" ref="N24" si="13">SQRT(L24/M24)</f>
         <v>0.10034945030122537</v>
       </c>
       <c r="O24" s="38">
-        <f t="shared" ref="O24" si="12">SQRT(L24*M24)</f>
+        <f t="shared" ref="O24" si="14">SQRT(L24*M24)</f>
         <v>5.017472515061268</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C25" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="86" t="s">
-        <v>109</v>
+      <c r="C25" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="83" t="s">
+        <v>105</v>
       </c>
       <c r="F25" s="44">
-        <v>-0.3</v>
+        <v>-1</v>
       </c>
       <c r="G25" s="44">
-        <v>-0.3</v>
+        <v>-1</v>
       </c>
       <c r="H25" s="44">
-        <v>-0.3</v>
-      </c>
-      <c r="I25" s="85" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I25" s="82" t="s">
         <v>3</v>
       </c>
       <c r="J25" s="44">
         <f>J22+F25</f>
-        <v>39.520000000000003</v>
+        <v>38.82</v>
       </c>
       <c r="K25" s="44"/>
       <c r="L25" s="38">
-        <f t="shared" si="7"/>
-        <v>8.9536476554959457</v>
+        <f t="shared" si="9"/>
+        <v>7.6207901002541334</v>
       </c>
       <c r="M25" s="38">
         <v>50</v>
       </c>
       <c r="N25" s="38">
-        <f t="shared" si="8"/>
-        <v>0.42317012313007035</v>
+        <f t="shared" si="10"/>
+        <v>0.39040466442536603</v>
       </c>
       <c r="O25" s="38">
-        <f t="shared" si="9"/>
-        <v>21.15850615650352</v>
+        <f t="shared" si="11"/>
+        <v>19.520233221268303</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.2">
@@ -4981,8 +5028,8 @@
       <c r="F28" s="44"/>
       <c r="G28" s="44"/>
       <c r="H28" s="44"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
+      <c r="L28" s="92"/>
+      <c r="M28" s="92"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.2">
       <c r="F29" s="45"/>
@@ -4991,82 +5038,82 @@
       <c r="L29" s="38">
         <v>50</v>
       </c>
-      <c r="M29" s="85" t="s">
-        <v>103</v>
-      </c>
-      <c r="N29" s="85"/>
+      <c r="M29" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="N29" s="82"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.2">
       <c r="E30" s="46" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F30" s="47">
         <f>SUM(F11:F26)</f>
-        <v>38.920000000000009</v>
+        <v>38.220000000000006</v>
       </c>
       <c r="G30" s="47">
         <f>SUM(G11:G26)</f>
-        <v>48.580000000000005</v>
+        <v>47.88</v>
       </c>
       <c r="H30" s="47">
         <f>SUM(H11:H26)</f>
-        <v>48.580000000000005</v>
+        <v>47.88</v>
       </c>
       <c r="I30" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="L30" s="85">
+      <c r="L30" s="82">
         <f>0.5*SQRT(2)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="N30" s="85"/>
+      <c r="N30" s="82"/>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E31" s="85" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31" s="87">
+      <c r="E31" s="82" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="84">
         <f>10^(F30/10)/1000</f>
-        <v>7.7983011052326132</v>
-      </c>
-      <c r="G31" s="87">
+        <v>6.6374307040191036</v>
+      </c>
+      <c r="G31" s="84">
         <f>10^(G30/10)/1000</f>
-        <v>72.110747918290102</v>
-      </c>
-      <c r="H31" s="87">
+        <v>61.376200516479472</v>
+      </c>
+      <c r="H31" s="84">
         <f>10^(H30/10)/1000</f>
-        <v>72.110747918290102</v>
-      </c>
-      <c r="I31" s="85" t="s">
-        <v>95</v>
+        <v>61.376200516479472</v>
+      </c>
+      <c r="I31" s="82" t="s">
+        <v>91</v>
       </c>
       <c r="L31" s="38">
         <f>L30/SQRT(2)</f>
         <v>0.5</v>
       </c>
-      <c r="N31" s="85"/>
+      <c r="N31" s="82"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.2">
       <c r="L32" s="38">
         <f>L31*L31/L29</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M32" s="85" t="s">
-        <v>102</v>
-      </c>
-      <c r="N32" s="85"/>
+      <c r="M32" s="82" t="s">
+        <v>98</v>
+      </c>
+      <c r="N32" s="82"/>
     </row>
     <row r="33" spans="6:13" x14ac:dyDescent="0.2">
       <c r="L33" s="38">
         <f>10*LOG10(L32)+30</f>
         <v>6.9897000433601875</v>
       </c>
-      <c r="M33" s="85" t="s">
+      <c r="M33" s="82" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="6:13" x14ac:dyDescent="0.2">
-      <c r="F35" s="85"/>
+      <c r="F35" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5078,27 +5125,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B5:F53"/>
+  <dimension ref="B5:F84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="99" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="83"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="95"/>
     </row>
     <row r="7" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="49" t="s">
@@ -5117,7 +5164,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="52">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="C8" s="53">
         <v>1.8</v>
@@ -5127,46 +5174,28 @@
       </c>
       <c r="E8" s="54">
         <f>C8*D8/B8</f>
-        <v>0.90423529411764703</v>
+        <v>0.76859999999999995</v>
       </c>
       <c r="F8" s="55" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="56">
-        <v>0.85</v>
-      </c>
-      <c r="C9" s="57">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="57">
-        <v>0.8</v>
-      </c>
-      <c r="E9" s="58">
-        <f t="shared" ref="E9:E17" si="0">C9*D9/B9</f>
-        <v>1.1294117647058823</v>
-      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="58"/>
       <c r="F9" s="51" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="56">
-        <v>0.85</v>
-      </c>
-      <c r="C10" s="57">
-        <v>3.3</v>
-      </c>
-      <c r="D10" s="57">
-        <v>1</v>
-      </c>
-      <c r="E10" s="58">
-        <f t="shared" si="0"/>
-        <v>3.8823529411764706</v>
-      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="51" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
@@ -5174,53 +5203,35 @@
         <v>1</v>
       </c>
       <c r="C11" s="57">
-        <v>5.5</v>
+        <v>1.2</v>
       </c>
       <c r="D11" s="57">
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="E11" s="58">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" ref="E11:E28" si="0">C11*D11/B11</f>
+        <v>0.96</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="56">
-        <v>1</v>
-      </c>
-      <c r="C12" s="57">
-        <v>5.5</v>
-      </c>
-      <c r="D12" s="57">
-        <v>0.5</v>
-      </c>
-      <c r="E12" s="58">
-        <f t="shared" si="0"/>
-        <v>2.75</v>
-      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="58"/>
       <c r="F12" s="51" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="56">
-        <v>1</v>
-      </c>
-      <c r="C13" s="57">
-        <v>5.5</v>
-      </c>
-      <c r="D13" s="57">
-        <v>2</v>
-      </c>
-      <c r="E13" s="58">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
+      <c r="B13" s="56"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
       <c r="F13" s="51" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
@@ -5228,71 +5239,44 @@
         <v>1</v>
       </c>
       <c r="C14" s="57">
-        <v>5.5</v>
+        <v>3.3</v>
       </c>
       <c r="D14" s="57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="58">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>3.3</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="56">
-        <v>1</v>
-      </c>
-      <c r="C15" s="57">
-        <v>5.5</v>
-      </c>
-      <c r="D15" s="57">
-        <v>0.1</v>
-      </c>
-      <c r="E15" s="58">
-        <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
-      </c>
+      <c r="B15" s="56"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="58"/>
       <c r="F15" s="51" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="56">
-        <v>1</v>
-      </c>
-      <c r="C16" s="57">
-        <v>5.5</v>
-      </c>
-      <c r="D16" s="57">
-        <v>0.1</v>
-      </c>
-      <c r="E16" s="58">
-        <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
-      </c>
+      <c r="B16" s="56"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="58"/>
       <c r="F16" s="51" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="56">
-        <v>1</v>
-      </c>
-      <c r="C17" s="57">
-        <v>5.5</v>
-      </c>
-      <c r="D17" s="57">
-        <v>1</v>
-      </c>
-      <c r="E17" s="58">
-        <f t="shared" si="0"/>
-        <v>5.5</v>
-      </c>
+      <c r="B17" s="56"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="58"/>
       <c r="F17" s="51" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
@@ -5300,84 +5284,134 @@
       <c r="C18" s="57"/>
       <c r="D18" s="57"/>
       <c r="E18" s="58"/>
-      <c r="F18" s="51"/>
+      <c r="F18" s="51" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="56"/>
       <c r="C19" s="57"/>
-      <c r="D19" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="58">
-        <f>SUM(E8:E17)</f>
-        <v>48.265999999999991</v>
-      </c>
-      <c r="F19" s="51"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="51" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="56"/>
       <c r="C20" s="57"/>
-      <c r="D20" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="58">
+      <c r="D20" s="57"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="56">
+        <v>1</v>
+      </c>
+      <c r="C21" s="57">
         <v>5.5</v>
       </c>
-      <c r="F20" s="51"/>
-    </row>
-    <row r="21" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="59"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="61">
-        <f>E19/E20</f>
-        <v>8.7756363636363623</v>
-      </c>
-      <c r="F21" s="62"/>
-    </row>
-    <row r="23" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+      <c r="D21" s="57">
+        <v>2</v>
+      </c>
+      <c r="E21" s="58">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F21" s="51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="56">
+        <v>1</v>
+      </c>
+      <c r="C22" s="57">
+        <v>5.5</v>
+      </c>
+      <c r="D22" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="58">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="F22" s="51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="56">
+        <v>1</v>
+      </c>
+      <c r="C23" s="57">
+        <v>5.5</v>
+      </c>
+      <c r="D23" s="57">
+        <v>2</v>
+      </c>
+      <c r="E23" s="58">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F23" s="51" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="81" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="82"/>
-      <c r="F24" s="83"/>
-    </row>
-    <row r="25" spans="2:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="65"/>
+      <c r="B24" s="56">
+        <v>1</v>
+      </c>
+      <c r="C24" s="57">
+        <v>5.5</v>
+      </c>
+      <c r="D24" s="57">
+        <v>2</v>
+      </c>
+      <c r="E24" s="58">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F24" s="51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="56">
+        <v>1</v>
+      </c>
+      <c r="C25" s="96">
+        <v>5.5</v>
+      </c>
+      <c r="D25" s="96">
+        <v>3</v>
+      </c>
+      <c r="E25" s="58">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+      <c r="F25" s="51" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="56">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="C26" s="57">
         <v>5.5</v>
       </c>
       <c r="D26" s="57">
-        <v>6.3</v>
+        <v>0.1</v>
       </c>
       <c r="E26" s="58">
-        <f t="shared" ref="E26:E28" si="1">C26*D26/B26</f>
-        <v>40.764705882352942</v>
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F26" s="51" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
@@ -5385,17 +5419,17 @@
         <v>1</v>
       </c>
       <c r="C27" s="57">
-        <v>29</v>
+        <v>5.5</v>
       </c>
       <c r="D27" s="57">
-        <v>1.8</v>
+        <v>0.1</v>
       </c>
       <c r="E27" s="58">
-        <f t="shared" si="1"/>
-        <v>52.2</v>
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F27" s="51" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
@@ -5403,17 +5437,17 @@
         <v>1</v>
       </c>
       <c r="C28" s="57">
-        <v>29</v>
+        <v>5.5</v>
       </c>
       <c r="D28" s="57">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="E28" s="58">
-        <f t="shared" si="1"/>
-        <v>52.2</v>
+        <f t="shared" si="0"/>
+        <v>5.5</v>
       </c>
       <c r="F28" s="51" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
@@ -5430,8 +5464,8 @@
         <v>44</v>
       </c>
       <c r="E30" s="58">
-        <f>SUM(E26:E28)</f>
-        <v>145.16470588235296</v>
+        <f>SUM(E8:E28)</f>
+        <v>63.878599999999992</v>
       </c>
       <c r="F30" s="51"/>
     </row>
@@ -5442,7 +5476,7 @@
         <v>42</v>
       </c>
       <c r="E31" s="58">
-        <v>29</v>
+        <v>5.5</v>
       </c>
       <c r="F31" s="51"/>
     </row>
@@ -5454,106 +5488,127 @@
       </c>
       <c r="E32" s="61">
         <f>E30/E31</f>
-        <v>5.0056795131845853</v>
+        <v>11.614290909090908</v>
       </c>
       <c r="F32" s="62"/>
     </row>
-    <row r="37" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="93" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="95"/>
+    </row>
+    <row r="36" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B36" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="51"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="52">
+        <v>1</v>
+      </c>
+      <c r="C37" s="53">
+        <v>3.7</v>
+      </c>
+      <c r="D37" s="53">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="E37" s="54">
+        <f>C37*D37/B37</f>
+        <v>0.49950000000000006</v>
+      </c>
+      <c r="F37" s="55" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="83"/>
-    </row>
-    <row r="39" spans="2:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B39" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="51"/>
+      <c r="B38" s="56">
+        <v>1</v>
+      </c>
+      <c r="C38" s="57">
+        <v>3.7</v>
+      </c>
+      <c r="D38" s="57">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="E38" s="58">
+        <f t="shared" ref="E38:E40" si="1">C38*D38/B38</f>
+        <v>1.9314000000000002</v>
+      </c>
+      <c r="F38" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="56">
+        <v>1</v>
+      </c>
+      <c r="C39" s="57">
+        <v>3.7</v>
+      </c>
+      <c r="D39" s="57">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="E39" s="58">
+        <f t="shared" si="1"/>
+        <v>2.4605000000000001</v>
+      </c>
+      <c r="F39" s="51" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="52">
+      <c r="B40" s="56">
         <v>1</v>
       </c>
-      <c r="C40" s="53">
+      <c r="C40" s="57">
         <v>3.7</v>
       </c>
-      <c r="D40" s="53">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="E40" s="54">
-        <f>C40*D40/B40</f>
-        <v>0.49950000000000006</v>
-      </c>
-      <c r="F40" s="55" t="s">
+      <c r="D40" s="57">
+        <v>0.435</v>
+      </c>
+      <c r="E40" s="58">
+        <f t="shared" si="1"/>
+        <v>1.6095000000000002</v>
+      </c>
+      <c r="F40" s="51" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="56">
-        <v>1</v>
-      </c>
-      <c r="C41" s="57">
-        <v>3.7</v>
-      </c>
-      <c r="D41" s="57">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="E41" s="58">
-        <f t="shared" ref="E41:E43" si="2">C41*D41/B41</f>
-        <v>1.9314000000000002</v>
-      </c>
-      <c r="F41" s="51" t="s">
-        <v>59</v>
-      </c>
+      <c r="B41" s="56"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="51"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="56">
-        <v>1</v>
-      </c>
-      <c r="C42" s="57">
-        <v>3.7</v>
-      </c>
-      <c r="D42" s="57">
-        <v>0.66500000000000004</v>
-      </c>
-      <c r="E42" s="58">
-        <f t="shared" si="2"/>
-        <v>2.4605000000000001</v>
-      </c>
-      <c r="F42" s="51" t="s">
-        <v>60</v>
-      </c>
+      <c r="B42" s="56"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="51"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="56">
-        <v>1</v>
-      </c>
-      <c r="C43" s="57">
-        <v>3.7</v>
-      </c>
-      <c r="D43" s="57">
-        <v>0.435</v>
-      </c>
-      <c r="E43" s="58">
-        <f t="shared" si="2"/>
-        <v>1.6095000000000002</v>
-      </c>
-      <c r="F43" s="51" t="s">
-        <v>61</v>
-      </c>
+      <c r="B43" s="56"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="51"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" s="56"/>
@@ -5586,64 +5641,341 @@
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" s="56"/>
       <c r="C48" s="57"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="58"/>
+      <c r="D48" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="58">
+        <f>SUM(E37:E46)</f>
+        <v>6.5009000000000015</v>
+      </c>
       <c r="F48" s="51"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" s="56"/>
       <c r="C49" s="57"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="58"/>
+      <c r="D49" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="58">
+        <v>3.9</v>
+      </c>
       <c r="F49" s="51"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B50" s="56"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="51"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="56"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57" t="s">
+    <row r="50" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="59"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="61">
+        <f>E48/E49</f>
+        <v>1.6668974358974362</v>
+      </c>
+      <c r="F50" s="62"/>
+    </row>
+    <row r="52" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B53" s="98" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" s="94"/>
+      <c r="D53" s="94"/>
+      <c r="E53" s="94"/>
+      <c r="F53" s="95"/>
+    </row>
+    <row r="54" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B54" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="58">
-        <f>SUM(E40:E49)</f>
-        <v>6.5009000000000015</v>
-      </c>
-      <c r="F51" s="51"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B52" s="56"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57" t="s">
+      <c r="F54" s="51"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B55" s="52"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="55"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B56" s="56"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="57"/>
+      <c r="E56" s="58"/>
+      <c r="F56" s="51"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B57" s="56"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="58"/>
+      <c r="F57" s="51"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B58" s="56"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="58"/>
+      <c r="F58" s="51"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B59" s="56"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="58"/>
+      <c r="F59" s="51"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B60" s="56"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="51"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B61" s="56"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="58"/>
+      <c r="F61" s="51"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B62" s="56"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="58"/>
+      <c r="F62" s="51"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B63" s="56"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="58"/>
+      <c r="F63" s="51"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B64" s="56"/>
+      <c r="C64" s="57"/>
+      <c r="D64" s="57"/>
+      <c r="E64" s="58"/>
+      <c r="F64" s="51"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B65" s="56"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="58"/>
+      <c r="F65" s="51"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" s="56"/>
+      <c r="C66" s="57"/>
+      <c r="D66" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="E66" s="58">
+        <f>SUM(E55:E64)</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="51"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" s="56"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="58">
+      <c r="E67" s="58">
         <v>3.9</v>
       </c>
-      <c r="F52" s="51"/>
-    </row>
-    <row r="53" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="59"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60" t="s">
+      <c r="F67" s="51"/>
+    </row>
+    <row r="68" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="59"/>
+      <c r="C68" s="60"/>
+      <c r="D68" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="E53" s="61">
-        <f>E51/E52</f>
+      <c r="E68" s="61">
+        <f>E66/E67</f>
+        <v>0</v>
+      </c>
+      <c r="F68" s="62"/>
+    </row>
+    <row r="73" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B74" s="93" t="s">
+        <v>52</v>
+      </c>
+      <c r="C74" s="94"/>
+      <c r="D74" s="94"/>
+      <c r="E74" s="94"/>
+      <c r="F74" s="95"/>
+    </row>
+    <row r="75" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B75" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="E75" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="F75" s="65"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B76" s="56">
+        <v>0.85</v>
+      </c>
+      <c r="C76" s="57">
+        <v>5.5</v>
+      </c>
+      <c r="D76" s="58">
+        <f>E32</f>
+        <v>11.614290909090908</v>
+      </c>
+      <c r="E76" s="58">
+        <f t="shared" ref="E76:E80" si="2">C76*D76/B76</f>
+        <v>75.151294117647055</v>
+      </c>
+      <c r="F76" s="51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B77" s="56">
+        <v>0.85</v>
+      </c>
+      <c r="C77" s="57">
+        <v>5.5</v>
+      </c>
+      <c r="D77" s="58">
+        <f>E50</f>
         <v>1.6668974358974362</v>
       </c>
-      <c r="F53" s="62"/>
+      <c r="E77" s="58">
+        <f t="shared" si="2"/>
+        <v>10.785806938159883</v>
+      </c>
+      <c r="F77" s="97" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B78" s="56">
+        <v>0.85</v>
+      </c>
+      <c r="C78" s="57">
+        <v>3.7</v>
+      </c>
+      <c r="D78" s="58">
+        <f>E68</f>
+        <v>0</v>
+      </c>
+      <c r="E78" s="58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F78" s="97" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B79" s="56">
+        <v>1</v>
+      </c>
+      <c r="C79" s="57">
+        <v>29</v>
+      </c>
+      <c r="D79" s="57">
+        <v>1</v>
+      </c>
+      <c r="E79" s="58">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="F79" s="51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B80" s="56">
+        <v>1</v>
+      </c>
+      <c r="C80" s="57">
+        <v>29</v>
+      </c>
+      <c r="D80" s="57">
+        <v>1</v>
+      </c>
+      <c r="E80" s="58">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="F80" s="51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B81" s="56"/>
+      <c r="C81" s="57"/>
+      <c r="D81" s="57"/>
+      <c r="E81" s="58"/>
+      <c r="F81" s="51"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B82" s="56"/>
+      <c r="C82" s="57"/>
+      <c r="D82" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="E82" s="58">
+        <f>SUM(E76:E80)</f>
+        <v>143.93710105580692</v>
+      </c>
+      <c r="F82" s="51"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B83" s="56"/>
+      <c r="C83" s="57"/>
+      <c r="D83" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="E83" s="58">
+        <v>29</v>
+      </c>
+      <c r="F83" s="51"/>
+    </row>
+    <row r="84" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="59"/>
+      <c r="C84" s="60"/>
+      <c r="D84" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" s="61">
+        <f>E82/E83</f>
+        <v>4.9633483122692041</v>
+      </c>
+      <c r="F84" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B53:F53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>